<commit_message>
12/14 - Fixes, Bowden extruder, and a gantry lock
- Fixed some issues with the left pulley component.
- Fixed an incorrect peg hole depth on right mid `XY Joint`.
- Added 5mm to the AB stepper mounts.
- Pushed Y limit switch out ~20mm to allow clearance for the X limit switch. This is hacky, but will work and keep the bed area available.
- Adjusted screw holes on right pulley component to account for the new limit switch mount.
- Designed Bowden mount for BMG.
- Designed `Gantry Lock` for servicing hotend and belts.
- Raised the Y limit switch a bit to give clearance for heated inserts in the mount.
</commit_message>
<xml_diff>
--- a/Docs/Printer Part Codes.xlsx
+++ b/Docs/Printer Part Codes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jon\Documents\3D Print\Clockmaker\Clock2\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jon\Documents\3D Print\Clockmaker\clock-3\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10E32109-14BB-4FF7-B20F-1A4A2729BA61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B43E88D2-2DF4-4E11-B349-8CDDBF60B26B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23436" yWindow="684" windowWidth="21468" windowHeight="11352" xr2:uid="{7E6554FF-2F4B-4318-87E0-43D225F4F170}"/>
+    <workbookView xWindow="23712" yWindow="960" windowWidth="21468" windowHeight="11352" xr2:uid="{7E6554FF-2F4B-4318-87E0-43D225F4F170}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="69">
   <si>
     <t>Component</t>
   </si>
@@ -223,6 +223,24 @@
   </si>
   <si>
     <t>?</t>
+  </si>
+  <si>
+    <t>STL Filename</t>
+  </si>
+  <si>
+    <t>Bowden Mount</t>
+  </si>
+  <si>
+    <t>BMG Bowden Mount</t>
+  </si>
+  <si>
+    <t>Bowden Coupler</t>
+  </si>
+  <si>
+    <t>Hotend adapter for bowden</t>
+  </si>
+  <si>
+    <t>Gantry Lock</t>
   </si>
 </sst>
 </file>
@@ -266,9 +284,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -287,8 +307,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5F341AE2-224B-4051-B04D-BA10CC5651EC}" name="Table1" displayName="Table1" ref="A1:H47" totalsRowShown="0">
-  <autoFilter ref="A1:H47" xr:uid="{7A633D33-D295-46C3-AB03-03E2AB6E078E}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5F341AE2-224B-4051-B04D-BA10CC5651EC}" name="Table1" displayName="Table1" ref="A1:I50" totalsRowShown="0">
+  <autoFilter ref="A1:I50" xr:uid="{7A633D33-D295-46C3-AB03-03E2AB6E078E}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -297,11 +317,12 @@
     <filterColumn colId="5" hiddenButton="1"/>
     <filterColumn colId="6" hiddenButton="1"/>
     <filterColumn colId="7" hiddenButton="1"/>
+    <filterColumn colId="8" hiddenButton="1"/>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H47">
-    <sortCondition ref="A1:A47"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I49">
+    <sortCondition ref="A1:A49"/>
   </sortState>
-  <tableColumns count="8">
+  <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{A8EA61BD-839A-4759-B873-CEDA7BEA684B}" name="Number"/>
     <tableColumn id="2" xr3:uid="{926BBC7C-2486-48E4-9BC6-985A230D6D2C}" name="Category"/>
     <tableColumn id="3" xr3:uid="{7E4828A1-DEFC-42E1-B49C-2FA9CE14DAFC}" name="Component"/>
@@ -309,6 +330,7 @@
     <tableColumn id="5" xr3:uid="{F485EE51-7281-43C9-BDF3-784C9FCF3319}" name="Name or Location"/>
     <tableColumn id="7" xr3:uid="{69C26183-B33F-4D8D-A901-9DFC879E5484}" name="Material"/>
     <tableColumn id="8" xr3:uid="{E02C7714-2483-4D13-AE3F-938B24F1DC26}" name="Qty"/>
+    <tableColumn id="9" xr3:uid="{2CDB0871-5B60-47E8-947B-D1E55965C018}" name="STL Filename"/>
     <tableColumn id="6" xr3:uid="{6584E548-497F-4E36-8AA8-8903B11B5D8A}" name="Note"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -612,10 +634,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CC8DB31-6D45-4FED-94B6-5390BD4B0F2C}">
-  <dimension ref="A1:H47"/>
+  <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="G48" sqref="G48"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H50" sqref="H50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -627,10 +649,11 @@
     <col min="5" max="5" width="20.5703125" customWidth="1"/>
     <col min="6" max="6" width="11.28515625" customWidth="1"/>
     <col min="7" max="7" width="5.42578125" customWidth="1"/>
-    <col min="8" max="8" width="21.42578125" customWidth="1"/>
+    <col min="8" max="8" width="13" customWidth="1"/>
+    <col min="9" max="9" width="26.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -653,11 +676,14 @@
         <v>61</v>
       </c>
       <c r="H1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
@@ -679,8 +705,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" t="s">
@@ -702,8 +728,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" t="s">
@@ -725,8 +751,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" t="s">
@@ -748,8 +774,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" t="s">
@@ -771,8 +797,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" t="s">
@@ -794,8 +820,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
         <v>7</v>
       </c>
       <c r="B8" t="s">
@@ -817,8 +843,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
         <v>8</v>
       </c>
       <c r="B9" t="s">
@@ -840,8 +866,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
         <v>9</v>
       </c>
       <c r="B10" t="s">
@@ -863,7 +889,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -886,7 +912,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -909,7 +935,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -932,7 +958,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -955,7 +981,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -978,7 +1004,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1001,7 +1027,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1024,7 +1050,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1047,7 +1073,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1069,11 +1095,11 @@
       <c r="G19">
         <v>1</v>
       </c>
-      <c r="H19" t="s">
+      <c r="I19" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1096,7 +1122,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1119,7 +1145,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1142,7 +1168,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1165,7 +1191,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1188,7 +1214,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1211,7 +1237,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1234,7 +1260,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1257,7 +1283,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1280,7 +1306,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1303,7 +1329,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1325,9 +1351,9 @@
       <c r="G30">
         <v>1</v>
       </c>
-      <c r="H30" s="1"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I30" s="1"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1349,9 +1375,9 @@
       <c r="G31">
         <v>1</v>
       </c>
-      <c r="H31" s="1"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I31" s="1"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1373,9 +1399,9 @@
       <c r="G32">
         <v>1</v>
       </c>
-      <c r="H32" s="1"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I32" s="1"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1397,9 +1423,9 @@
       <c r="G33">
         <v>1</v>
       </c>
-      <c r="H33" s="1"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I33" s="1"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1421,9 +1447,9 @@
       <c r="G34">
         <v>1</v>
       </c>
-      <c r="H34" s="1"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I34" s="1"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1446,7 +1472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1469,7 +1495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>41</v>
       </c>
@@ -1492,7 +1518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>42</v>
       </c>
@@ -1515,7 +1541,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>43</v>
       </c>
@@ -1538,7 +1564,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>44</v>
       </c>
@@ -1561,7 +1587,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>45</v>
       </c>
@@ -1584,7 +1610,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>51</v>
       </c>
@@ -1607,79 +1633,80 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B43" t="s">
         <v>48</v>
       </c>
       <c r="C43" t="s">
+        <v>66</v>
+      </c>
+      <c r="D43" t="s">
+        <v>1</v>
+      </c>
+      <c r="E43" t="s">
+        <v>66</v>
+      </c>
+      <c r="F43" t="s">
+        <v>57</v>
+      </c>
+      <c r="I43" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>61</v>
+      </c>
+      <c r="B44" t="s">
+        <v>48</v>
+      </c>
+      <c r="C44" t="s">
         <v>50</v>
       </c>
-      <c r="D43" t="s">
-        <v>1</v>
-      </c>
-      <c r="E43" t="s">
+      <c r="D44" t="s">
+        <v>1</v>
+      </c>
+      <c r="E44" t="s">
         <v>49</v>
       </c>
-      <c r="F43" t="s">
-        <v>57</v>
-      </c>
-      <c r="G43">
-        <v>1</v>
-      </c>
-      <c r="H43" s="1"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44">
+      <c r="F44" t="s">
+        <v>57</v>
+      </c>
+      <c r="G44">
+        <v>1</v>
+      </c>
+      <c r="I44" s="1"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>62</v>
+      </c>
+      <c r="B45" t="s">
+        <v>48</v>
+      </c>
+      <c r="C45" t="s">
+        <v>64</v>
+      </c>
+      <c r="D45" t="s">
+        <v>1</v>
+      </c>
+      <c r="E45" t="s">
+        <v>65</v>
+      </c>
+      <c r="F45" t="s">
+        <v>57</v>
+      </c>
+      <c r="G45">
+        <v>1</v>
+      </c>
+      <c r="I45" s="1"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46">
         <v>90</v>
-      </c>
-      <c r="B44" t="s">
-        <v>38</v>
-      </c>
-      <c r="C44" t="s">
-        <v>41</v>
-      </c>
-      <c r="D44" t="s">
-        <v>1</v>
-      </c>
-      <c r="E44" t="s">
-        <v>39</v>
-      </c>
-      <c r="F44" t="s">
-        <v>57</v>
-      </c>
-      <c r="G44" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>91</v>
-      </c>
-      <c r="B45" t="s">
-        <v>38</v>
-      </c>
-      <c r="C45" t="s">
-        <v>25</v>
-      </c>
-      <c r="D45" t="s">
-        <v>1</v>
-      </c>
-      <c r="E45" t="s">
-        <v>40</v>
-      </c>
-      <c r="F45" t="s">
-        <v>57</v>
-      </c>
-      <c r="G45">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>92</v>
       </c>
       <c r="B46" t="s">
         <v>38</v>
@@ -1691,36 +1718,105 @@
         <v>1</v>
       </c>
       <c r="E46" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F46" t="s">
-        <v>37</v>
-      </c>
-      <c r="G46">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="G46" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B47" t="s">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="C47" t="s">
         <v>25</v>
       </c>
       <c r="D47" t="s">
+        <v>1</v>
+      </c>
+      <c r="E47" t="s">
+        <v>40</v>
+      </c>
+      <c r="F47" t="s">
+        <v>57</v>
+      </c>
+      <c r="G47">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>92</v>
+      </c>
+      <c r="B48" t="s">
+        <v>38</v>
+      </c>
+      <c r="C48" t="s">
+        <v>41</v>
+      </c>
+      <c r="D48" t="s">
+        <v>1</v>
+      </c>
+      <c r="E48" t="s">
+        <v>42</v>
+      </c>
+      <c r="F48" t="s">
+        <v>37</v>
+      </c>
+      <c r="G48">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>93</v>
+      </c>
+      <c r="B49" t="s">
+        <v>4</v>
+      </c>
+      <c r="C49" t="s">
+        <v>25</v>
+      </c>
+      <c r="D49" t="s">
         <v>9</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E49" t="s">
         <v>60</v>
       </c>
-      <c r="F47" t="s">
-        <v>57</v>
-      </c>
-      <c r="G47">
-        <v>1</v>
+      <c r="F49" t="s">
+        <v>57</v>
+      </c>
+      <c r="G49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>94</v>
+      </c>
+      <c r="B50" t="s">
+        <v>38</v>
+      </c>
+      <c r="C50" t="s">
+        <v>25</v>
+      </c>
+      <c r="D50" t="s">
+        <v>1</v>
+      </c>
+      <c r="E50" t="s">
+        <v>68</v>
+      </c>
+      <c r="F50" t="s">
+        <v>57</v>
+      </c>
+      <c r="G50">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2021/12/15 - Mostly wiring
- Tested XY motion
- Designed and tested replacement for Z bottom bracket that includes rail alignment.
- Tested all endstops
- Added build plate
- Sketched up panel mounts for JST-SM connectors for 2-6 pins and fit-tested
- Began setting up wiring for JST-SM
- Added STL Filename column to `Part Codes`
- Crimped a lot of wires.
- Created file for tracking wire codes and terminal names
</commit_message>
<xml_diff>
--- a/Docs/Printer Part Codes.xlsx
+++ b/Docs/Printer Part Codes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jon\Documents\3D Print\Clockmaker\clock-3\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B43E88D2-2DF4-4E11-B349-8CDDBF60B26B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C891AF68-A94F-4FAD-87AA-40C38E14CA98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23712" yWindow="960" windowWidth="21468" windowHeight="11352" xr2:uid="{7E6554FF-2F4B-4318-87E0-43D225F4F170}"/>
+    <workbookView xWindow="24264" yWindow="1512" windowWidth="21468" windowHeight="11352" xr2:uid="{7E6554FF-2F4B-4318-87E0-43D225F4F170}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="119">
   <si>
     <t>Component</t>
   </si>
@@ -132,9 +132,6 @@
     <t>XY Joint</t>
   </si>
   <si>
-    <t>Linear Rail Stop</t>
-  </si>
-  <si>
     <t>Hotend</t>
   </si>
   <si>
@@ -241,6 +238,159 @@
   </si>
   <si>
     <t>Gantry Lock</t>
+  </si>
+  <si>
+    <t>Tools</t>
+  </si>
+  <si>
+    <t>Lower Rail Bracket</t>
+  </si>
+  <si>
+    <t>01 - XY - Pulleys - L Bottom.stl</t>
+  </si>
+  <si>
+    <t>02 - XY - Pulleys - L Top.stl</t>
+  </si>
+  <si>
+    <t>05 - XY - XY Joint - L Top.stl</t>
+  </si>
+  <si>
+    <t>06 - XY - XY Joint - L Mid.stl</t>
+  </si>
+  <si>
+    <t>07 - XY - XY Joint - L Bottom.stl</t>
+  </si>
+  <si>
+    <t>03 - XY - Pulleys - R Bottom.stl</t>
+  </si>
+  <si>
+    <t>04 - XY - Pulleys - R Top.stl</t>
+  </si>
+  <si>
+    <t>08 - XY - XY Joint - R Top.stl</t>
+  </si>
+  <si>
+    <t>09 - XY - XY Joint - R Mid.stl</t>
+  </si>
+  <si>
+    <t>10 - XY - XY Joint - R Bottom.stl</t>
+  </si>
+  <si>
+    <t>11 - XY - Tensioner - Bolt Receiver.stl</t>
+  </si>
+  <si>
+    <t>12 - XY - Tensioner - Idler Seat.stl</t>
+  </si>
+  <si>
+    <t>13 - XY - Tensioner - Tensioner Cap.stl</t>
+  </si>
+  <si>
+    <t>14 - XY - Tensioner - Guide Frame.stl</t>
+  </si>
+  <si>
+    <t>15 - XY - Steppers - Bearing Support Plate.stl</t>
+  </si>
+  <si>
+    <t>16 - XY - Steppers - Stepper Mount.stl</t>
+  </si>
+  <si>
+    <t>17 - XY - Motion - L Y Axis Rail Guide.stl</t>
+  </si>
+  <si>
+    <t>18 - XY - Motion - R Y Axis Rail Guide.stl</t>
+  </si>
+  <si>
+    <t>19 - Z - Motion - Lower Rail Bracket.stl</t>
+  </si>
+  <si>
+    <t>20 - Z - Bed - Corner Bracket.stl</t>
+  </si>
+  <si>
+    <t>21 - Z - Motion - L Gantry.stl</t>
+  </si>
+  <si>
+    <t>22 - Z - Motion - R Gantry.stl</t>
+  </si>
+  <si>
+    <t>23 - Z - Steppers - L Stepper Mount.stl</t>
+  </si>
+  <si>
+    <t>24 - Z - Steppers - R Stepper Mount.stl</t>
+  </si>
+  <si>
+    <t>25 - Z - Motion - L Z1 Limit Switch.stl</t>
+  </si>
+  <si>
+    <t>26 - Z - Motion - R Z2 Limit Switch.stl</t>
+  </si>
+  <si>
+    <t>27 - Z - Motion - L Lead Screw Plate.stl</t>
+  </si>
+  <si>
+    <t>28 - Z - Motion - R Lead Screw Plate.stl</t>
+  </si>
+  <si>
+    <t>29 - Z - Bed - Wire Support.stl</t>
+  </si>
+  <si>
+    <t>30 - X Gantry - Carriage Mount.stl</t>
+  </si>
+  <si>
+    <t>31 - X Gantry - Top Mount.stl</t>
+  </si>
+  <si>
+    <t>32 - X Gantry - Back Plate.stl</t>
+  </si>
+  <si>
+    <t>33 - X Gantry - Front Plate.stl</t>
+  </si>
+  <si>
+    <t>34 - Gantry - Carriage - L Belt Clamp.stl</t>
+  </si>
+  <si>
+    <t>35 - Gantry - Carriage - R Belt Clamp.stl</t>
+  </si>
+  <si>
+    <t>40 - X Gantry - Hotend - Mounting Bracket.stl</t>
+  </si>
+  <si>
+    <t>41 - X Gantry - Hotend - Locking Collar.stl</t>
+  </si>
+  <si>
+    <t>42 - X Gantry - Hotend - Fan Intake.stl</t>
+  </si>
+  <si>
+    <t>43 - X Gantry - Hotend - PTFE Collar (TPU).stl</t>
+  </si>
+  <si>
+    <t>44 - Gantry - Hotend  - EVA Duct.stl</t>
+  </si>
+  <si>
+    <t>45 - Gantry - Hotend - Fan Mount.stl</t>
+  </si>
+  <si>
+    <t>51 - ABL - Mount - BLTouch.stl</t>
+  </si>
+  <si>
+    <t>61 - Extruder - Mount - BMG.stl</t>
+  </si>
+  <si>
+    <t>62 - Extruder - Bowden Mount - Bowden BMG Mount.stl</t>
+  </si>
+  <si>
+    <t>90 - Misc - Bracket Cover.stl</t>
+  </si>
+  <si>
+    <t>91 - Misc - Limit Switch Cap.stl</t>
+  </si>
+  <si>
+    <t>92 - Misc - Frame Base Foot (TPU).stl</t>
+  </si>
+  <si>
+    <t>93 - XY - Motion - X Limit Switch Mount.stl</t>
+  </si>
+  <si>
+    <t>94 - Misc - Tools - Gantry Lock.stl</t>
   </si>
 </sst>
 </file>
@@ -330,8 +480,8 @@
     <tableColumn id="5" xr3:uid="{F485EE51-7281-43C9-BDF3-784C9FCF3319}" name="Name or Location"/>
     <tableColumn id="7" xr3:uid="{69C26183-B33F-4D8D-A901-9DFC879E5484}" name="Material"/>
     <tableColumn id="8" xr3:uid="{E02C7714-2483-4D13-AE3F-938B24F1DC26}" name="Qty"/>
+    <tableColumn id="6" xr3:uid="{6584E548-497F-4E36-8AA8-8903B11B5D8A}" name="Note"/>
     <tableColumn id="9" xr3:uid="{2CDB0871-5B60-47E8-947B-D1E55965C018}" name="STL Filename"/>
-    <tableColumn id="6" xr3:uid="{6584E548-497F-4E36-8AA8-8903B11B5D8A}" name="Note"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -636,21 +786,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CC8DB31-6D45-4FED-94B6-5390BD4B0F2C}">
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H50" sqref="H50"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.42578125" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
     <col min="4" max="4" width="13.42578125" customWidth="1"/>
     <col min="5" max="5" width="20.5703125" customWidth="1"/>
     <col min="6" max="6" width="11.28515625" customWidth="1"/>
     <col min="7" max="7" width="5.42578125" customWidth="1"/>
-    <col min="8" max="8" width="13" customWidth="1"/>
-    <col min="9" max="9" width="26.28515625" customWidth="1"/>
+    <col min="8" max="8" width="26.28515625" customWidth="1"/>
+    <col min="9" max="9" width="48.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -670,16 +820,16 @@
         <v>20</v>
       </c>
       <c r="F1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H1" t="s">
-        <v>63</v>
+        <v>30</v>
       </c>
       <c r="I1" t="s">
-        <v>30</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -699,10 +849,13 @@
         <v>7</v>
       </c>
       <c r="F2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G2">
         <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -722,10 +875,13 @@
         <v>8</v>
       </c>
       <c r="F3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G3">
         <v>1</v>
+      </c>
+      <c r="I3" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -745,10 +901,13 @@
         <v>7</v>
       </c>
       <c r="F4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G4">
         <v>1</v>
+      </c>
+      <c r="I4" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -768,10 +927,13 @@
         <v>8</v>
       </c>
       <c r="F5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G5">
         <v>1</v>
+      </c>
+      <c r="I5" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -791,10 +953,13 @@
         <v>8</v>
       </c>
       <c r="F6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G6">
         <v>1</v>
+      </c>
+      <c r="I6" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -814,10 +979,13 @@
         <v>10</v>
       </c>
       <c r="F7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G7">
         <v>1</v>
+      </c>
+      <c r="I7" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -837,10 +1005,13 @@
         <v>7</v>
       </c>
       <c r="F8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G8">
         <v>1</v>
+      </c>
+      <c r="I8" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -860,10 +1031,13 @@
         <v>8</v>
       </c>
       <c r="F9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G9">
         <v>1</v>
+      </c>
+      <c r="I9" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -883,10 +1057,13 @@
         <v>10</v>
       </c>
       <c r="F10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G10">
         <v>1</v>
+      </c>
+      <c r="I10" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -906,10 +1083,13 @@
         <v>7</v>
       </c>
       <c r="F11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G11">
         <v>1</v>
+      </c>
+      <c r="I11" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -929,10 +1109,13 @@
         <v>12</v>
       </c>
       <c r="F12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G12">
         <v>2</v>
+      </c>
+      <c r="I12" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -952,10 +1135,13 @@
         <v>13</v>
       </c>
       <c r="F13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G13">
         <v>2</v>
+      </c>
+      <c r="I13" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -975,10 +1161,13 @@
         <v>14</v>
       </c>
       <c r="F14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G14">
         <v>2</v>
+      </c>
+      <c r="I14" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -998,10 +1187,13 @@
         <v>15</v>
       </c>
       <c r="F15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G15">
         <v>2</v>
+      </c>
+      <c r="I15" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1021,10 +1213,13 @@
         <v>17</v>
       </c>
       <c r="F16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G16">
         <v>2</v>
+      </c>
+      <c r="I16" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -1044,10 +1239,13 @@
         <v>18</v>
       </c>
       <c r="F17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G17">
         <v>2</v>
+      </c>
+      <c r="I17" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1064,13 +1262,16 @@
         <v>5</v>
       </c>
       <c r="E18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G18">
         <v>1</v>
+      </c>
+      <c r="I18" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1087,16 +1288,19 @@
         <v>9</v>
       </c>
       <c r="E19" t="s">
+        <v>57</v>
+      </c>
+      <c r="F19" t="s">
+        <v>56</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19" t="s">
         <v>58</v>
       </c>
-      <c r="F19" t="s">
-        <v>57</v>
-      </c>
-      <c r="G19">
-        <v>1</v>
-      </c>
       <c r="I19" t="s">
-        <v>59</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1113,13 +1317,16 @@
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>32</v>
+        <v>69</v>
       </c>
       <c r="F20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G20">
         <v>2</v>
+      </c>
+      <c r="I20" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1139,10 +1346,13 @@
         <v>23</v>
       </c>
       <c r="F21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G21">
         <v>4</v>
+      </c>
+      <c r="I21" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1162,10 +1372,13 @@
         <v>24</v>
       </c>
       <c r="F22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G22">
         <v>1</v>
+      </c>
+      <c r="I22" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -1185,10 +1398,13 @@
         <v>24</v>
       </c>
       <c r="F23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G23">
         <v>1</v>
+      </c>
+      <c r="I23" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -1208,10 +1424,13 @@
         <v>18</v>
       </c>
       <c r="F24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G24">
         <v>1</v>
+      </c>
+      <c r="I24" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -1231,10 +1450,13 @@
         <v>18</v>
       </c>
       <c r="F25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G25">
         <v>1</v>
+      </c>
+      <c r="I25" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -1254,10 +1476,13 @@
         <v>26</v>
       </c>
       <c r="F26" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G26">
         <v>1</v>
+      </c>
+      <c r="I26" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -1277,10 +1502,13 @@
         <v>27</v>
       </c>
       <c r="F27" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G27">
         <v>1</v>
+      </c>
+      <c r="I27" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -1300,10 +1528,13 @@
         <v>28</v>
       </c>
       <c r="F28" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G28">
         <v>1</v>
+      </c>
+      <c r="I28" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -1323,10 +1554,13 @@
         <v>28</v>
       </c>
       <c r="F29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G29">
         <v>1</v>
+      </c>
+      <c r="I29" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -1346,12 +1580,15 @@
         <v>29</v>
       </c>
       <c r="F30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G30">
         <v>1</v>
       </c>
-      <c r="I30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
@@ -1361,21 +1598,24 @@
         <v>24</v>
       </c>
       <c r="C31" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D31" t="s">
         <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F31" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G31">
         <v>1</v>
       </c>
-      <c r="I31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
@@ -1385,21 +1625,24 @@
         <v>24</v>
       </c>
       <c r="C32" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D32" t="s">
         <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F32" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G32">
         <v>1</v>
       </c>
-      <c r="I32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
@@ -1409,21 +1652,24 @@
         <v>24</v>
       </c>
       <c r="C33" t="s">
+        <v>43</v>
+      </c>
+      <c r="D33" t="s">
+        <v>1</v>
+      </c>
+      <c r="E33" t="s">
         <v>44</v>
       </c>
-      <c r="D33" t="s">
-        <v>1</v>
-      </c>
-      <c r="E33" t="s">
-        <v>45</v>
-      </c>
       <c r="F33" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G33">
         <v>1</v>
       </c>
-      <c r="I33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
@@ -1433,21 +1679,24 @@
         <v>24</v>
       </c>
       <c r="C34" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D34" t="s">
         <v>1</v>
       </c>
       <c r="E34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F34" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G34">
         <v>1</v>
       </c>
-      <c r="I34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
@@ -1457,19 +1706,22 @@
         <v>24</v>
       </c>
       <c r="C35" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D35" t="s">
         <v>5</v>
       </c>
       <c r="E35" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F35" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G35">
         <v>1</v>
+      </c>
+      <c r="I35" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -1480,19 +1732,22 @@
         <v>24</v>
       </c>
       <c r="C36" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D36" t="s">
         <v>9</v>
       </c>
       <c r="E36" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F36" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G36">
         <v>1</v>
+      </c>
+      <c r="I36" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -1503,19 +1758,22 @@
         <v>24</v>
       </c>
       <c r="C37" t="s">
+        <v>32</v>
+      </c>
+      <c r="D37" t="s">
+        <v>1</v>
+      </c>
+      <c r="E37" t="s">
         <v>33</v>
       </c>
-      <c r="D37" t="s">
-        <v>1</v>
-      </c>
-      <c r="E37" t="s">
-        <v>34</v>
-      </c>
       <c r="F37" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G37">
         <v>1</v>
+      </c>
+      <c r="I37" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -1526,19 +1784,22 @@
         <v>24</v>
       </c>
       <c r="C38" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D38" t="s">
         <v>1</v>
       </c>
       <c r="E38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G38">
         <v>1</v>
+      </c>
+      <c r="I38" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -1549,19 +1810,22 @@
         <v>24</v>
       </c>
       <c r="C39" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D39" t="s">
         <v>1</v>
       </c>
       <c r="E39" t="s">
+        <v>35</v>
+      </c>
+      <c r="F39" t="s">
         <v>36</v>
       </c>
-      <c r="F39" t="s">
-        <v>37</v>
-      </c>
       <c r="G39">
         <v>1</v>
+      </c>
+      <c r="I39" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -1572,19 +1836,22 @@
         <v>24</v>
       </c>
       <c r="C40" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D40" t="s">
         <v>1</v>
       </c>
       <c r="E40" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F40" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G40">
         <v>1</v>
+      </c>
+      <c r="I40" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -1595,19 +1862,22 @@
         <v>24</v>
       </c>
       <c r="C41" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D41" t="s">
         <v>1</v>
       </c>
       <c r="E41" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F41" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G41">
         <v>1</v>
+      </c>
+      <c r="I41" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -1615,22 +1885,25 @@
         <v>51</v>
       </c>
       <c r="B42" t="s">
+        <v>50</v>
+      </c>
+      <c r="C42" t="s">
+        <v>49</v>
+      </c>
+      <c r="D42" t="s">
+        <v>1</v>
+      </c>
+      <c r="E42" t="s">
         <v>51</v>
       </c>
-      <c r="C42" t="s">
-        <v>50</v>
-      </c>
-      <c r="D42" t="s">
-        <v>1</v>
-      </c>
-      <c r="E42" t="s">
-        <v>52</v>
-      </c>
       <c r="F42" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G42">
         <v>1</v>
+      </c>
+      <c r="I42" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -1638,22 +1911,28 @@
         <v>60</v>
       </c>
       <c r="B43" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C43" t="s">
+        <v>65</v>
+      </c>
+      <c r="D43" t="s">
+        <v>1</v>
+      </c>
+      <c r="E43" t="s">
+        <v>65</v>
+      </c>
+      <c r="F43" t="s">
+        <v>56</v>
+      </c>
+      <c r="G43">
+        <v>1</v>
+      </c>
+      <c r="H43" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D43" t="s">
-        <v>1</v>
-      </c>
-      <c r="E43" t="s">
-        <v>66</v>
-      </c>
-      <c r="F43" t="s">
-        <v>57</v>
-      </c>
-      <c r="I43" s="3" t="s">
-        <v>67</v>
+      <c r="I43" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -1661,70 +1940,79 @@
         <v>61</v>
       </c>
       <c r="B44" t="s">
+        <v>47</v>
+      </c>
+      <c r="C44" t="s">
+        <v>49</v>
+      </c>
+      <c r="D44" t="s">
+        <v>1</v>
+      </c>
+      <c r="E44" t="s">
         <v>48</v>
       </c>
-      <c r="C44" t="s">
-        <v>50</v>
-      </c>
-      <c r="D44" t="s">
-        <v>1</v>
-      </c>
-      <c r="E44" t="s">
-        <v>49</v>
-      </c>
       <c r="F44" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G44">
         <v>1</v>
       </c>
-      <c r="I44" s="1"/>
+      <c r="H44" s="1"/>
+      <c r="I44" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>62</v>
       </c>
       <c r="B45" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C45" t="s">
+        <v>63</v>
+      </c>
+      <c r="D45" t="s">
+        <v>1</v>
+      </c>
+      <c r="E45" t="s">
         <v>64</v>
       </c>
-      <c r="D45" t="s">
-        <v>1</v>
-      </c>
-      <c r="E45" t="s">
-        <v>65</v>
-      </c>
       <c r="F45" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G45">
         <v>1</v>
       </c>
-      <c r="I45" s="1"/>
+      <c r="H45" s="1"/>
+      <c r="I45" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>90</v>
       </c>
       <c r="B46" t="s">
+        <v>37</v>
+      </c>
+      <c r="C46" t="s">
+        <v>40</v>
+      </c>
+      <c r="D46" t="s">
+        <v>1</v>
+      </c>
+      <c r="E46" t="s">
         <v>38</v>
       </c>
-      <c r="C46" t="s">
-        <v>41</v>
-      </c>
-      <c r="D46" t="s">
-        <v>1</v>
-      </c>
-      <c r="E46" t="s">
-        <v>39</v>
-      </c>
       <c r="F46" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G46" t="s">
-        <v>62</v>
+        <v>61</v>
+      </c>
+      <c r="I46" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
@@ -1732,7 +2020,7 @@
         <v>91</v>
       </c>
       <c r="B47" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C47" t="s">
         <v>25</v>
@@ -1741,13 +2029,16 @@
         <v>1</v>
       </c>
       <c r="E47" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F47" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G47">
         <v>5</v>
+      </c>
+      <c r="I47" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -1755,25 +2046,28 @@
         <v>92</v>
       </c>
       <c r="B48" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C48" t="s">
+        <v>40</v>
+      </c>
+      <c r="D48" t="s">
+        <v>1</v>
+      </c>
+      <c r="E48" t="s">
         <v>41</v>
       </c>
-      <c r="D48" t="s">
-        <v>1</v>
-      </c>
-      <c r="E48" t="s">
-        <v>42</v>
-      </c>
       <c r="F48" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G48">
         <v>4</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I48" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>93</v>
       </c>
@@ -1787,36 +2081,42 @@
         <v>9</v>
       </c>
       <c r="E49" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F49" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G49">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I49" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>94</v>
       </c>
       <c r="B50" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C50" t="s">
-        <v>25</v>
+        <v>68</v>
       </c>
       <c r="D50" t="s">
         <v>1</v>
       </c>
       <c r="E50" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F50" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G50">
         <v>2</v>
+      </c>
+      <c r="I50" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2021/12/18 - Fixes and board mounts
- Fixed emboss on right patch panel
- Revision 2 of XY Joint wire guide. Dealing with some elephant's foot.
- Added a file for extending spare T slot underneath for mounting equipment. The file is parametric for the end-user's modification.
- Designed clamps for board mounting
- Added screw holes to board tray to secure it in place.
- Modified blank tray template and exported STEP file to `/CAD` folder.
- Rebuilt Octopus tray from template file.
- Threw out the last four entries about clamps and boards and went with a simpler design with fewer parts and easier mounting.
- Boards mount at an angle for easier access from the front.
- Made parts for both Octopus and SKR 2 (1.4 if you can find it anymore)
- Started plotting out Octopus fan header usage (cleaner and simpler for now than using SKR 2 + bucks)
</commit_message>
<xml_diff>
--- a/Docs/Printer Part Codes.xlsx
+++ b/Docs/Printer Part Codes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jon\Documents\3D Print\Clockmaker\clock-3\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CE4A5A5-D9ED-49AE-A8D9-54C7F2F81640}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD5D8764-2B56-4ACC-ABCE-FD767242FA40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{7E6554FF-2F4B-4318-87E0-43D225F4F170}"/>
+    <workbookView xWindow="23256" yWindow="72" windowWidth="22236" windowHeight="13200" xr2:uid="{7E6554FF-2F4B-4318-87E0-43D225F4F170}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="146">
   <si>
     <t>Component</t>
   </si>
@@ -435,13 +435,43 @@
     <t>95 - Misc - Wiring - Wire Guide.stl</t>
   </si>
   <si>
-    <t>Wire Anchor</t>
-  </si>
-  <si>
-    <t>96 - Misc - Wiring - Wire Anchor.stl</t>
-  </si>
-  <si>
     <t>Still Testing</t>
+  </si>
+  <si>
+    <t>Control Board Clamp</t>
+  </si>
+  <si>
+    <t>Board Tray</t>
+  </si>
+  <si>
+    <t>Octopus Board Tray</t>
+  </si>
+  <si>
+    <t>78 - Electrical - Board Tray - Octopus Board Tray.stl</t>
+  </si>
+  <si>
+    <t>77 - Electrical - Mount - R Control Board Clamp.stl</t>
+  </si>
+  <si>
+    <t>76 - Electrical - Mount - L Control Board Clamp.stl</t>
+  </si>
+  <si>
+    <t>SKR Board Tray</t>
+  </si>
+  <si>
+    <t>79 - Electrical - Board Tray - SKR Board Tray.stl</t>
+  </si>
+  <si>
+    <t>96 - Misc - Wiring - T Slot Wire Anchor.stl</t>
+  </si>
+  <si>
+    <t>T Slot Wire Anchor</t>
+  </si>
+  <si>
+    <t>XY Joint Wire Guide</t>
+  </si>
+  <si>
+    <t>97 - Misc - Wiring - R XY Joint Wire Guide.stl</t>
   </si>
 </sst>
 </file>
@@ -508,8 +538,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5F341AE2-224B-4051-B04D-BA10CC5651EC}" name="Table1" displayName="Table1" ref="A1:I58" totalsRowShown="0">
-  <autoFilter ref="A1:I58" xr:uid="{7A633D33-D295-46C3-AB03-03E2AB6E078E}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5F341AE2-224B-4051-B04D-BA10CC5651EC}" name="Table1" displayName="Table1" ref="A1:I63" totalsRowShown="0">
+  <autoFilter ref="A1:I63" xr:uid="{7A633D33-D295-46C3-AB03-03E2AB6E078E}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -520,8 +550,8 @@
     <filterColumn colId="7" hiddenButton="1"/>
     <filterColumn colId="8" hiddenButton="1"/>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I56">
-    <sortCondition ref="A1:A56"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I62">
+    <sortCondition ref="A1:A62"/>
   </sortState>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{A8EA61BD-839A-4759-B873-CEDA7BEA684B}" name="Number"/>
@@ -835,10 +865,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CC8DB31-6D45-4FED-94B6-5390BD4B0F2C}">
-  <dimension ref="A1:I58"/>
+  <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H62" sqref="H62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2204,97 +2234,97 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="B52" t="s">
-        <v>37</v>
+        <v>119</v>
       </c>
       <c r="C52" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="D52" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E52" t="s">
-        <v>38</v>
+        <v>134</v>
       </c>
       <c r="F52" t="s">
         <v>56</v>
       </c>
-      <c r="G52" t="s">
-        <v>61</v>
+      <c r="G52">
+        <v>1</v>
       </c>
       <c r="I52" t="s">
-        <v>114</v>
+        <v>139</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="B53" t="s">
-        <v>37</v>
+        <v>119</v>
       </c>
       <c r="C53" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="D53" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E53" t="s">
-        <v>39</v>
+        <v>134</v>
       </c>
       <c r="F53" t="s">
         <v>56</v>
       </c>
       <c r="G53">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I53" t="s">
-        <v>115</v>
+        <v>138</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="B54" t="s">
-        <v>37</v>
+        <v>119</v>
       </c>
       <c r="C54" t="s">
-        <v>40</v>
+        <v>135</v>
       </c>
       <c r="D54" t="s">
         <v>1</v>
       </c>
       <c r="E54" t="s">
-        <v>41</v>
+        <v>136</v>
       </c>
       <c r="F54" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="G54">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I54" t="s">
-        <v>116</v>
+        <v>137</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="B55" t="s">
-        <v>4</v>
+        <v>119</v>
       </c>
       <c r="C55" t="s">
-        <v>25</v>
+        <v>135</v>
       </c>
       <c r="D55" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E55" t="s">
-        <v>59</v>
+        <v>140</v>
       </c>
       <c r="F55" t="s">
         <v>56</v>
@@ -2303,88 +2333,218 @@
         <v>1</v>
       </c>
       <c r="I55" t="s">
-        <v>117</v>
+        <v>141</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B56" t="s">
         <v>37</v>
       </c>
       <c r="C56" t="s">
-        <v>68</v>
+        <v>40</v>
       </c>
       <c r="D56" t="s">
         <v>1</v>
       </c>
       <c r="E56" t="s">
-        <v>67</v>
+        <v>38</v>
       </c>
       <c r="F56" t="s">
         <v>56</v>
       </c>
-      <c r="G56">
-        <v>2</v>
+      <c r="G56" t="s">
+        <v>61</v>
       </c>
       <c r="I56" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B57" t="s">
         <v>37</v>
       </c>
       <c r="C57" t="s">
-        <v>120</v>
+        <v>25</v>
       </c>
       <c r="D57" t="s">
         <v>1</v>
       </c>
       <c r="E57" t="s">
-        <v>131</v>
+        <v>39</v>
       </c>
       <c r="F57" t="s">
-        <v>36</v>
-      </c>
-      <c r="G57" t="s">
-        <v>61</v>
-      </c>
-      <c r="H57" t="s">
-        <v>135</v>
+        <v>56</v>
+      </c>
+      <c r="G57">
+        <v>5</v>
       </c>
       <c r="I57" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B58" t="s">
         <v>37</v>
       </c>
       <c r="C58" t="s">
+        <v>40</v>
+      </c>
+      <c r="D58" t="s">
+        <v>1</v>
+      </c>
+      <c r="E58" t="s">
+        <v>41</v>
+      </c>
+      <c r="F58" t="s">
+        <v>36</v>
+      </c>
+      <c r="G58">
+        <v>4</v>
+      </c>
+      <c r="I58" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>93</v>
+      </c>
+      <c r="B59" t="s">
+        <v>4</v>
+      </c>
+      <c r="C59" t="s">
+        <v>25</v>
+      </c>
+      <c r="D59" t="s">
+        <v>9</v>
+      </c>
+      <c r="E59" t="s">
+        <v>59</v>
+      </c>
+      <c r="F59" t="s">
+        <v>56</v>
+      </c>
+      <c r="G59">
+        <v>1</v>
+      </c>
+      <c r="I59" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>94</v>
+      </c>
+      <c r="B60" t="s">
+        <v>37</v>
+      </c>
+      <c r="C60" t="s">
+        <v>68</v>
+      </c>
+      <c r="D60" t="s">
+        <v>1</v>
+      </c>
+      <c r="E60" t="s">
+        <v>67</v>
+      </c>
+      <c r="F60" t="s">
+        <v>56</v>
+      </c>
+      <c r="G60">
+        <v>2</v>
+      </c>
+      <c r="I60" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>95</v>
+      </c>
+      <c r="B61" t="s">
+        <v>37</v>
+      </c>
+      <c r="C61" t="s">
         <v>120</v>
       </c>
-      <c r="D58" t="s">
-        <v>1</v>
-      </c>
-      <c r="E58" t="s">
+      <c r="D61" t="s">
+        <v>1</v>
+      </c>
+      <c r="E61" t="s">
+        <v>131</v>
+      </c>
+      <c r="F61" t="s">
+        <v>36</v>
+      </c>
+      <c r="G61" t="s">
+        <v>61</v>
+      </c>
+      <c r="H61" t="s">
         <v>133</v>
       </c>
-      <c r="F58" t="s">
-        <v>56</v>
-      </c>
-      <c r="G58">
+      <c r="I61" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>96</v>
+      </c>
+      <c r="B62" t="s">
+        <v>37</v>
+      </c>
+      <c r="C62" t="s">
+        <v>120</v>
+      </c>
+      <c r="D62" t="s">
+        <v>1</v>
+      </c>
+      <c r="E62" t="s">
+        <v>143</v>
+      </c>
+      <c r="F62" t="s">
+        <v>56</v>
+      </c>
+      <c r="G62">
         <v>10</v>
       </c>
-      <c r="I58" t="s">
-        <v>134</v>
+      <c r="I62" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>97</v>
+      </c>
+      <c r="B63" t="s">
+        <v>37</v>
+      </c>
+      <c r="C63" t="s">
+        <v>120</v>
+      </c>
+      <c r="D63" t="s">
+        <v>9</v>
+      </c>
+      <c r="E63" t="s">
+        <v>144</v>
+      </c>
+      <c r="F63" t="s">
+        <v>56</v>
+      </c>
+      <c r="G63">
+        <v>1</v>
+      </c>
+      <c r="I63" t="s">
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
12/19 - T Slot Extensions and removed gantry lock
- Recrimped (properly) all but three of the JST SM connections. Generic crimper for the XH and PH connectors arrived, so went ahead and finished the connectors for all three harnesses above the electrical undercarriage.
- Created an 80mm fan mount for cooling the steppers. Will upload after verifying the second print fits.
- Mounted the Octopus.
- Started work on skirt layout, including IEC (power in) and power switch location.
- Crimped even more wires.
</commit_message>
<xml_diff>
--- a/Docs/Printer Part Codes.xlsx
+++ b/Docs/Printer Part Codes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jon\Documents\3D Print\Clockmaker\clock-3\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD5D8764-2B56-4ACC-ABCE-FD767242FA40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96EE668D-903B-4540-992D-4793E3E42A9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23256" yWindow="72" windowWidth="22236" windowHeight="13200" xr2:uid="{7E6554FF-2F4B-4318-87E0-43D225F4F170}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="150">
   <si>
     <t>Component</t>
   </si>
@@ -438,30 +439,12 @@
     <t>Still Testing</t>
   </si>
   <si>
-    <t>Control Board Clamp</t>
-  </si>
-  <si>
     <t>Board Tray</t>
   </si>
   <si>
-    <t>Octopus Board Tray</t>
-  </si>
-  <si>
-    <t>78 - Electrical - Board Tray - Octopus Board Tray.stl</t>
-  </si>
-  <si>
-    <t>77 - Electrical - Mount - R Control Board Clamp.stl</t>
-  </si>
-  <si>
-    <t>76 - Electrical - Mount - L Control Board Clamp.stl</t>
-  </si>
-  <si>
     <t>SKR Board Tray</t>
   </si>
   <si>
-    <t>79 - Electrical - Board Tray - SKR Board Tray.stl</t>
-  </si>
-  <si>
     <t>96 - Misc - Wiring - T Slot Wire Anchor.stl</t>
   </si>
   <si>
@@ -472,6 +455,36 @@
   </si>
   <si>
     <t>97 - Misc - Wiring - R XY Joint Wire Guide.stl</t>
+  </si>
+  <si>
+    <t>Octopus Board Mount</t>
+  </si>
+  <si>
+    <t>77 - Electrical - Mount - R Octopus Board Mount.stl</t>
+  </si>
+  <si>
+    <t>76 - Electrical - Mount - L Octopus Board Mount.stl</t>
+  </si>
+  <si>
+    <t>78 - Electrical - Mount - L SKR Board Mount.stl</t>
+  </si>
+  <si>
+    <t>79 - Electrical - Mount - R SKR Board Mount.stl</t>
+  </si>
+  <si>
+    <t>80mm Fan Mount</t>
+  </si>
+  <si>
+    <t>Fan Grill</t>
+  </si>
+  <si>
+    <t>80mm Fan Grill</t>
+  </si>
+  <si>
+    <t>81 - Electrical - Fan Grill - 80mm Fan Grill.stl</t>
+  </si>
+  <si>
+    <t>80 - Electrical - Fan Mount - 80mm Fan Mount.stl</t>
   </si>
 </sst>
 </file>
@@ -538,8 +551,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5F341AE2-224B-4051-B04D-BA10CC5651EC}" name="Table1" displayName="Table1" ref="A1:I63" totalsRowShown="0">
-  <autoFilter ref="A1:I63" xr:uid="{7A633D33-D295-46C3-AB03-03E2AB6E078E}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5F341AE2-224B-4051-B04D-BA10CC5651EC}" name="Table1" displayName="Table1" ref="A1:I65" totalsRowShown="0">
+  <autoFilter ref="A1:I65" xr:uid="{7A633D33-D295-46C3-AB03-03E2AB6E078E}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -550,8 +563,8 @@
     <filterColumn colId="7" hiddenButton="1"/>
     <filterColumn colId="8" hiddenButton="1"/>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I62">
-    <sortCondition ref="A1:A62"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I64">
+    <sortCondition ref="A1:A64"/>
   </sortState>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{A8EA61BD-839A-4759-B873-CEDA7BEA684B}" name="Number"/>
@@ -865,10 +878,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CC8DB31-6D45-4FED-94B6-5390BD4B0F2C}">
-  <dimension ref="A1:I63"/>
+  <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H62" sqref="H62"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H63" sqref="H63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2246,7 +2259,7 @@
         <v>5</v>
       </c>
       <c r="E52" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="F52" t="s">
         <v>56</v>
@@ -2255,7 +2268,7 @@
         <v>1</v>
       </c>
       <c r="I52" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
@@ -2272,7 +2285,7 @@
         <v>9</v>
       </c>
       <c r="E53" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="F53" t="s">
         <v>56</v>
@@ -2281,7 +2294,7 @@
         <v>1</v>
       </c>
       <c r="I53" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
@@ -2292,14 +2305,14 @@
         <v>119</v>
       </c>
       <c r="C54" t="s">
+        <v>134</v>
+      </c>
+      <c r="D54" t="s">
+        <v>5</v>
+      </c>
+      <c r="E54" t="s">
         <v>135</v>
       </c>
-      <c r="D54" t="s">
-        <v>1</v>
-      </c>
-      <c r="E54" t="s">
-        <v>136</v>
-      </c>
       <c r="F54" t="s">
         <v>56</v>
       </c>
@@ -2307,7 +2320,7 @@
         <v>1</v>
       </c>
       <c r="I54" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
@@ -2318,14 +2331,14 @@
         <v>119</v>
       </c>
       <c r="C55" t="s">
+        <v>134</v>
+      </c>
+      <c r="D55" t="s">
+        <v>9</v>
+      </c>
+      <c r="E55" t="s">
         <v>135</v>
       </c>
-      <c r="D55" t="s">
-        <v>1</v>
-      </c>
-      <c r="E55" t="s">
-        <v>140</v>
-      </c>
       <c r="F55" t="s">
         <v>56</v>
       </c>
@@ -2333,64 +2346,64 @@
         <v>1</v>
       </c>
       <c r="I55" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="B56" t="s">
-        <v>37</v>
+        <v>119</v>
       </c>
       <c r="C56" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="D56" t="s">
         <v>1</v>
       </c>
       <c r="E56" t="s">
-        <v>38</v>
+        <v>145</v>
       </c>
       <c r="F56" t="s">
         <v>56</v>
       </c>
-      <c r="G56" t="s">
-        <v>61</v>
+      <c r="G56">
+        <v>1</v>
       </c>
       <c r="I56" t="s">
-        <v>114</v>
+        <v>149</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="B57" t="s">
-        <v>37</v>
+        <v>119</v>
       </c>
       <c r="C57" t="s">
-        <v>25</v>
+        <v>146</v>
       </c>
       <c r="D57" t="s">
         <v>1</v>
       </c>
       <c r="E57" t="s">
-        <v>39</v>
+        <v>147</v>
       </c>
       <c r="F57" t="s">
         <v>56</v>
       </c>
       <c r="G57">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I57" t="s">
-        <v>115</v>
+        <v>148</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B58" t="s">
         <v>37</v>
@@ -2402,128 +2415,128 @@
         <v>1</v>
       </c>
       <c r="E58" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F58" t="s">
-        <v>36</v>
-      </c>
-      <c r="G58">
-        <v>4</v>
+        <v>56</v>
+      </c>
+      <c r="G58" t="s">
+        <v>61</v>
       </c>
       <c r="I58" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B59" t="s">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="C59" t="s">
         <v>25</v>
       </c>
       <c r="D59" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E59" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="F59" t="s">
         <v>56</v>
       </c>
       <c r="G59">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I59" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B60" t="s">
         <v>37</v>
       </c>
       <c r="C60" t="s">
-        <v>68</v>
+        <v>40</v>
       </c>
       <c r="D60" t="s">
         <v>1</v>
       </c>
       <c r="E60" t="s">
-        <v>67</v>
+        <v>41</v>
       </c>
       <c r="F60" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="G60">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I60" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B61" t="s">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="C61" t="s">
-        <v>120</v>
+        <v>25</v>
       </c>
       <c r="D61" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E61" t="s">
-        <v>131</v>
+        <v>59</v>
       </c>
       <c r="F61" t="s">
-        <v>36</v>
-      </c>
-      <c r="G61" t="s">
-        <v>61</v>
-      </c>
-      <c r="H61" t="s">
-        <v>133</v>
+        <v>56</v>
+      </c>
+      <c r="G61">
+        <v>1</v>
       </c>
       <c r="I61" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B62" t="s">
         <v>37</v>
       </c>
       <c r="C62" t="s">
-        <v>120</v>
+        <v>68</v>
       </c>
       <c r="D62" t="s">
         <v>1</v>
       </c>
       <c r="E62" t="s">
-        <v>143</v>
+        <v>67</v>
       </c>
       <c r="F62" t="s">
         <v>56</v>
       </c>
       <c r="G62">
-        <v>10</v>
+        <v>2</v>
+      </c>
+      <c r="H62" t="s">
+        <v>133</v>
       </c>
       <c r="I62" t="s">
-        <v>142</v>
+        <v>118</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B63" t="s">
         <v>37</v>
@@ -2532,19 +2545,74 @@
         <v>120</v>
       </c>
       <c r="D63" t="s">
+        <v>1</v>
+      </c>
+      <c r="E63" t="s">
+        <v>131</v>
+      </c>
+      <c r="F63" t="s">
+        <v>36</v>
+      </c>
+      <c r="G63" t="s">
+        <v>61</v>
+      </c>
+      <c r="H63" t="s">
+        <v>133</v>
+      </c>
+      <c r="I63" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>96</v>
+      </c>
+      <c r="B64" t="s">
+        <v>37</v>
+      </c>
+      <c r="C64" t="s">
+        <v>120</v>
+      </c>
+      <c r="D64" t="s">
+        <v>1</v>
+      </c>
+      <c r="E64" t="s">
+        <v>137</v>
+      </c>
+      <c r="F64" t="s">
+        <v>56</v>
+      </c>
+      <c r="G64">
+        <v>10</v>
+      </c>
+      <c r="I64" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>97</v>
+      </c>
+      <c r="B65" t="s">
+        <v>37</v>
+      </c>
+      <c r="C65" t="s">
+        <v>120</v>
+      </c>
+      <c r="D65" t="s">
         <v>9</v>
       </c>
-      <c r="E63" t="s">
-        <v>144</v>
-      </c>
-      <c r="F63" t="s">
-        <v>56</v>
-      </c>
-      <c r="G63">
-        <v>1</v>
-      </c>
-      <c r="I63" t="s">
-        <v>145</v>
+      <c r="E65" t="s">
+        <v>138</v>
+      </c>
+      <c r="F65" t="s">
+        <v>56</v>
+      </c>
+      <c r="G65">
+        <v>1</v>
+      </c>
+      <c r="I65" t="s">
+        <v>139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
12/22 - RPi Mount, Marlin Config
- Preparing for vacation, so slowing activity.
- Significantly cleaned up wiring in undercarriage area.
- Added Marlin firmware modifications to source tree. Eventually switching to Klipper, but this is functional.
- Slight modification to the SKR2 board mount to improve clearance beneath.
- Created a Raspberry Pi board mount.
</commit_message>
<xml_diff>
--- a/Docs/Printer Part Codes.xlsx
+++ b/Docs/Printer Part Codes.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jon\Documents\3D Print\Clockmaker\clock-3\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D97CA42-DD9C-4B34-B5CD-D002425A6A60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5E01710-6FF8-483F-B8BF-6838D362F44E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23256" yWindow="72" windowWidth="22236" windowHeight="13200" xr2:uid="{7E6554FF-2F4B-4318-87E0-43D225F4F170}"/>
+    <workbookView xWindow="23256" yWindow="0" windowWidth="22236" windowHeight="12960" xr2:uid="{7E6554FF-2F4B-4318-87E0-43D225F4F170}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="158">
   <si>
     <t>Component</t>
   </si>
@@ -439,9 +438,6 @@
     <t>Still Testing</t>
   </si>
   <si>
-    <t>Board Tray</t>
-  </si>
-  <si>
     <t>SKR Board Tray</t>
   </si>
   <si>
@@ -503,6 +499,15 @@
   </si>
   <si>
     <t>LED Guide, 12mm</t>
+  </si>
+  <si>
+    <t>RPi Board Mount</t>
+  </si>
+  <si>
+    <t>83 - Electrical - Mount - L RPi Board Mount.stl</t>
+  </si>
+  <si>
+    <t>84 - Electrical - Mount - R RPi Board Mount.stl</t>
   </si>
 </sst>
 </file>
@@ -569,8 +574,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5F341AE2-224B-4051-B04D-BA10CC5651EC}" name="Table1" displayName="Table1" ref="A1:I67" totalsRowShown="0">
-  <autoFilter ref="A1:I67" xr:uid="{7A633D33-D295-46C3-AB03-03E2AB6E078E}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5F341AE2-224B-4051-B04D-BA10CC5651EC}" name="Table1" displayName="Table1" ref="A1:I69" totalsRowShown="0">
+  <autoFilter ref="A1:I69" xr:uid="{7A633D33-D295-46C3-AB03-03E2AB6E078E}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -581,8 +586,8 @@
     <filterColumn colId="7" hiddenButton="1"/>
     <filterColumn colId="8" hiddenButton="1"/>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I65">
-    <sortCondition ref="A1:A65"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I67">
+    <sortCondition ref="A1:A67"/>
   </sortState>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{A8EA61BD-839A-4759-B873-CEDA7BEA684B}" name="Number"/>
@@ -896,10 +901,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CC8DB31-6D45-4FED-94B6-5390BD4B0F2C}">
-  <dimension ref="A1:I67"/>
+  <dimension ref="A1:I69"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E59" sqref="E59"/>
+      <selection activeCell="I60" sqref="I60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2277,7 +2282,7 @@
         <v>5</v>
       </c>
       <c r="E52" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F52" t="s">
         <v>56</v>
@@ -2286,7 +2291,7 @@
         <v>1</v>
       </c>
       <c r="I52" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
@@ -2303,16 +2308,16 @@
         <v>9</v>
       </c>
       <c r="E53" t="s">
+        <v>139</v>
+      </c>
+      <c r="F53" t="s">
+        <v>56</v>
+      </c>
+      <c r="G53">
+        <v>1</v>
+      </c>
+      <c r="I53" t="s">
         <v>140</v>
-      </c>
-      <c r="F53" t="s">
-        <v>56</v>
-      </c>
-      <c r="G53">
-        <v>1</v>
-      </c>
-      <c r="I53" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
@@ -2323,13 +2328,13 @@
         <v>119</v>
       </c>
       <c r="C54" t="s">
-        <v>134</v>
+        <v>49</v>
       </c>
       <c r="D54" t="s">
         <v>5</v>
       </c>
       <c r="E54" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F54" t="s">
         <v>56</v>
@@ -2338,7 +2343,7 @@
         <v>1</v>
       </c>
       <c r="I54" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
@@ -2349,13 +2354,13 @@
         <v>119</v>
       </c>
       <c r="C55" t="s">
-        <v>134</v>
+        <v>49</v>
       </c>
       <c r="D55" t="s">
         <v>9</v>
       </c>
       <c r="E55" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F55" t="s">
         <v>56</v>
@@ -2364,7 +2369,7 @@
         <v>1</v>
       </c>
       <c r="I55" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
@@ -2381,7 +2386,7 @@
         <v>1</v>
       </c>
       <c r="E56" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F56" t="s">
         <v>56</v>
@@ -2390,7 +2395,7 @@
         <v>1</v>
       </c>
       <c r="I56" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
@@ -2401,22 +2406,22 @@
         <v>119</v>
       </c>
       <c r="C57" t="s">
+        <v>145</v>
+      </c>
+      <c r="D57" t="s">
+        <v>1</v>
+      </c>
+      <c r="E57" t="s">
         <v>146</v>
       </c>
-      <c r="D57" t="s">
-        <v>1</v>
-      </c>
-      <c r="E57" t="s">
+      <c r="F57" t="s">
+        <v>56</v>
+      </c>
+      <c r="G57">
+        <v>1</v>
+      </c>
+      <c r="I57" t="s">
         <v>147</v>
-      </c>
-      <c r="F57" t="s">
-        <v>56</v>
-      </c>
-      <c r="G57">
-        <v>1</v>
-      </c>
-      <c r="I57" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
@@ -2427,82 +2432,82 @@
         <v>119</v>
       </c>
       <c r="C58" t="s">
+        <v>151</v>
+      </c>
+      <c r="D58" t="s">
+        <v>1</v>
+      </c>
+      <c r="E58" t="s">
+        <v>154</v>
+      </c>
+      <c r="F58" t="s">
+        <v>56</v>
+      </c>
+      <c r="G58">
+        <v>1</v>
+      </c>
+      <c r="H58" t="s">
         <v>152</v>
       </c>
-      <c r="D58" t="s">
-        <v>1</v>
-      </c>
-      <c r="E58" t="s">
-        <v>155</v>
-      </c>
-      <c r="F58" t="s">
-        <v>56</v>
-      </c>
-      <c r="G58">
-        <v>3</v>
-      </c>
-      <c r="H58" t="s">
+      <c r="I58" t="s">
         <v>153</v>
-      </c>
-      <c r="I58" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B59" t="s">
-        <v>37</v>
+        <v>119</v>
       </c>
       <c r="C59" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="D59" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E59" t="s">
-        <v>38</v>
+        <v>155</v>
       </c>
       <c r="F59" t="s">
         <v>56</v>
       </c>
-      <c r="G59" t="s">
-        <v>61</v>
+      <c r="G59">
+        <v>1</v>
       </c>
       <c r="I59" t="s">
-        <v>114</v>
+        <v>156</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="B60" t="s">
-        <v>37</v>
+        <v>119</v>
       </c>
       <c r="C60" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="D60" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E60" t="s">
-        <v>39</v>
+        <v>155</v>
       </c>
       <c r="F60" t="s">
         <v>56</v>
       </c>
       <c r="G60">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I60" t="s">
-        <v>115</v>
+        <v>157</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B61" t="s">
         <v>37</v>
@@ -2514,131 +2519,128 @@
         <v>1</v>
       </c>
       <c r="E61" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F61" t="s">
-        <v>36</v>
-      </c>
-      <c r="G61">
-        <v>4</v>
+        <v>56</v>
+      </c>
+      <c r="G61" t="s">
+        <v>61</v>
       </c>
       <c r="I61" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B62" t="s">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="C62" t="s">
         <v>25</v>
       </c>
       <c r="D62" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E62" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="F62" t="s">
         <v>56</v>
       </c>
       <c r="G62">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I62" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B63" t="s">
         <v>37</v>
       </c>
       <c r="C63" t="s">
-        <v>68</v>
+        <v>40</v>
       </c>
       <c r="D63" t="s">
         <v>1</v>
       </c>
       <c r="E63" t="s">
-        <v>67</v>
+        <v>41</v>
       </c>
       <c r="F63" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="G63">
-        <v>2</v>
-      </c>
-      <c r="H63" t="s">
-        <v>133</v>
+        <v>4</v>
       </c>
       <c r="I63" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B64" t="s">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="C64" t="s">
-        <v>120</v>
+        <v>25</v>
       </c>
       <c r="D64" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E64" t="s">
-        <v>131</v>
+        <v>59</v>
       </c>
       <c r="F64" t="s">
-        <v>36</v>
-      </c>
-      <c r="G64" t="s">
-        <v>61</v>
-      </c>
-      <c r="H64" t="s">
-        <v>133</v>
+        <v>56</v>
+      </c>
+      <c r="G64">
+        <v>1</v>
       </c>
       <c r="I64" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B65" t="s">
         <v>37</v>
       </c>
       <c r="C65" t="s">
-        <v>120</v>
+        <v>68</v>
       </c>
       <c r="D65" t="s">
         <v>1</v>
       </c>
       <c r="E65" t="s">
-        <v>137</v>
+        <v>67</v>
       </c>
       <c r="F65" t="s">
         <v>56</v>
       </c>
       <c r="G65">
-        <v>10</v>
+        <v>2</v>
+      </c>
+      <c r="H65" t="s">
+        <v>133</v>
       </c>
       <c r="I65" t="s">
-        <v>136</v>
+        <v>118</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B66" t="s">
         <v>37</v>
@@ -2647,24 +2649,27 @@
         <v>120</v>
       </c>
       <c r="D66" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E66" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="F66" t="s">
-        <v>56</v>
-      </c>
-      <c r="G66">
-        <v>1</v>
+        <v>36</v>
+      </c>
+      <c r="G66" t="s">
+        <v>61</v>
+      </c>
+      <c r="H66" t="s">
+        <v>133</v>
       </c>
       <c r="I66" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B67" t="s">
         <v>37</v>
@@ -2676,16 +2681,68 @@
         <v>1</v>
       </c>
       <c r="E67" t="s">
+        <v>136</v>
+      </c>
+      <c r="F67" t="s">
+        <v>56</v>
+      </c>
+      <c r="G67">
+        <v>10</v>
+      </c>
+      <c r="I67" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>97</v>
+      </c>
+      <c r="B68" t="s">
+        <v>37</v>
+      </c>
+      <c r="C68" t="s">
+        <v>120</v>
+      </c>
+      <c r="D68" t="s">
+        <v>9</v>
+      </c>
+      <c r="E68" t="s">
+        <v>137</v>
+      </c>
+      <c r="F68" t="s">
+        <v>56</v>
+      </c>
+      <c r="G68">
+        <v>1</v>
+      </c>
+      <c r="I68" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>98</v>
+      </c>
+      <c r="B69" t="s">
+        <v>37</v>
+      </c>
+      <c r="C69" t="s">
+        <v>120</v>
+      </c>
+      <c r="D69" t="s">
+        <v>1</v>
+      </c>
+      <c r="E69" t="s">
+        <v>149</v>
+      </c>
+      <c r="F69" t="s">
+        <v>56</v>
+      </c>
+      <c r="G69">
+        <v>1</v>
+      </c>
+      <c r="I69" t="s">
         <v>150</v>
-      </c>
-      <c r="F67" t="s">
-        <v>56</v>
-      </c>
-      <c r="G67">
-        <v>1</v>
-      </c>
-      <c r="I67" t="s">
-        <v>151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
12/23 - Buck Mount added
Added #85 for a DROK 5A buck converter.
</commit_message>
<xml_diff>
--- a/Docs/Printer Part Codes.xlsx
+++ b/Docs/Printer Part Codes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jon\Documents\3D Print\Clockmaker\clock-3\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5E01710-6FF8-483F-B8BF-6838D362F44E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9205F57C-A4EA-4E11-8B09-E5B6EA4F2357}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23256" yWindow="0" windowWidth="22236" windowHeight="12960" xr2:uid="{7E6554FF-2F4B-4318-87E0-43D225F4F170}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="160">
   <si>
     <t>Component</t>
   </si>
@@ -508,6 +508,12 @@
   </si>
   <si>
     <t>84 - Electrical - Mount - R RPi Board Mount.stl</t>
+  </si>
+  <si>
+    <t>5A Buck Mount</t>
+  </si>
+  <si>
+    <t>85 - Electrical - Mount - 5A Buck Mount.stl</t>
   </si>
 </sst>
 </file>
@@ -574,8 +580,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5F341AE2-224B-4051-B04D-BA10CC5651EC}" name="Table1" displayName="Table1" ref="A1:I69" totalsRowShown="0">
-  <autoFilter ref="A1:I69" xr:uid="{7A633D33-D295-46C3-AB03-03E2AB6E078E}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5F341AE2-224B-4051-B04D-BA10CC5651EC}" name="Table1" displayName="Table1" ref="A1:I70" totalsRowShown="0">
+  <autoFilter ref="A1:I70" xr:uid="{7A633D33-D295-46C3-AB03-03E2AB6E078E}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -586,8 +592,8 @@
     <filterColumn colId="7" hiddenButton="1"/>
     <filterColumn colId="8" hiddenButton="1"/>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I67">
-    <sortCondition ref="A1:A67"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I68">
+    <sortCondition ref="A1:A68"/>
   </sortState>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{A8EA61BD-839A-4759-B873-CEDA7BEA684B}" name="Number"/>
@@ -901,10 +907,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CC8DB31-6D45-4FED-94B6-5390BD4B0F2C}">
-  <dimension ref="A1:I69"/>
+  <dimension ref="A1:I70"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I60" sqref="I60"/>
+      <selection activeCell="I61" sqref="I61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2507,169 +2513,166 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B61" t="s">
-        <v>37</v>
+        <v>119</v>
       </c>
       <c r="C61" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="D61" t="s">
         <v>1</v>
       </c>
       <c r="E61" t="s">
-        <v>38</v>
+        <v>158</v>
       </c>
       <c r="F61" t="s">
         <v>56</v>
       </c>
-      <c r="G61" t="s">
-        <v>61</v>
+      <c r="G61">
+        <v>1</v>
       </c>
       <c r="I61" t="s">
-        <v>114</v>
+        <v>159</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B62" t="s">
         <v>37</v>
       </c>
       <c r="C62" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="D62" t="s">
         <v>1</v>
       </c>
       <c r="E62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F62" t="s">
         <v>56</v>
       </c>
-      <c r="G62">
-        <v>5</v>
+      <c r="G62" t="s">
+        <v>61</v>
       </c>
       <c r="I62" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B63" t="s">
         <v>37</v>
       </c>
       <c r="C63" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="D63" t="s">
         <v>1</v>
       </c>
       <c r="E63" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F63" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="G63">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I63" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B64" t="s">
+        <v>37</v>
+      </c>
+      <c r="C64" t="s">
+        <v>40</v>
+      </c>
+      <c r="D64" t="s">
+        <v>1</v>
+      </c>
+      <c r="E64" t="s">
+        <v>41</v>
+      </c>
+      <c r="F64" t="s">
+        <v>36</v>
+      </c>
+      <c r="G64">
         <v>4</v>
       </c>
-      <c r="C64" t="s">
-        <v>25</v>
-      </c>
-      <c r="D64" t="s">
-        <v>9</v>
-      </c>
-      <c r="E64" t="s">
-        <v>59</v>
-      </c>
-      <c r="F64" t="s">
-        <v>56</v>
-      </c>
-      <c r="G64">
-        <v>1</v>
-      </c>
       <c r="I64" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B65" t="s">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="C65" t="s">
-        <v>68</v>
+        <v>25</v>
       </c>
       <c r="D65" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E65" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="F65" t="s">
         <v>56</v>
       </c>
       <c r="G65">
-        <v>2</v>
-      </c>
-      <c r="H65" t="s">
-        <v>133</v>
+        <v>1</v>
       </c>
       <c r="I65" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B66" t="s">
         <v>37</v>
       </c>
       <c r="C66" t="s">
-        <v>120</v>
+        <v>68</v>
       </c>
       <c r="D66" t="s">
         <v>1</v>
       </c>
       <c r="E66" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="F66" t="s">
-        <v>36</v>
-      </c>
-      <c r="G66" t="s">
-        <v>61</v>
+        <v>56</v>
+      </c>
+      <c r="G66">
+        <v>2</v>
       </c>
       <c r="H66" t="s">
         <v>133</v>
       </c>
       <c r="I66" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B67" t="s">
         <v>37</v>
@@ -2681,21 +2684,24 @@
         <v>1</v>
       </c>
       <c r="E67" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="F67" t="s">
-        <v>56</v>
-      </c>
-      <c r="G67">
-        <v>10</v>
+        <v>36</v>
+      </c>
+      <c r="G67" t="s">
+        <v>61</v>
+      </c>
+      <c r="H67" t="s">
+        <v>133</v>
       </c>
       <c r="I67" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B68" t="s">
         <v>37</v>
@@ -2704,24 +2710,24 @@
         <v>120</v>
       </c>
       <c r="D68" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E68" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F68" t="s">
         <v>56</v>
       </c>
       <c r="G68">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="I68" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B69" t="s">
         <v>37</v>
@@ -2730,18 +2736,44 @@
         <v>120</v>
       </c>
       <c r="D69" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E69" t="s">
+        <v>137</v>
+      </c>
+      <c r="F69" t="s">
+        <v>56</v>
+      </c>
+      <c r="G69">
+        <v>1</v>
+      </c>
+      <c r="I69" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>98</v>
+      </c>
+      <c r="B70" t="s">
+        <v>37</v>
+      </c>
+      <c r="C70" t="s">
+        <v>120</v>
+      </c>
+      <c r="D70" t="s">
+        <v>1</v>
+      </c>
+      <c r="E70" t="s">
         <v>149</v>
       </c>
-      <c r="F69" t="s">
-        <v>56</v>
-      </c>
-      <c r="G69">
-        <v>1</v>
-      </c>
-      <c r="I69" t="s">
+      <c r="F70" t="s">
+        <v>56</v>
+      </c>
+      <c r="G70">
+        <v>1</v>
+      </c>
+      <c r="I70" t="s">
         <v>150</v>
       </c>
     </row>

</xml_diff>

<commit_message>
12-26 - Frame caps
- Significant work done on skirts:
- Designed frame and section system. Front panels are modular and replaceable but fit together with screws.
- Finished 92mm fan intake, right switch panel, two identical center grille pieces.
- Work for screen and front communications ports can be done once back in office.
- Rear panel has two grilles and two fan cutouts, plus an IEC panel mount spot.
- Not entirely satisfied with fan cutouts, will work on them in the morning and push everything tomorrow.
- Added #s 100-103, the caps to cover the exterior frame edges at the base and top.
</commit_message>
<xml_diff>
--- a/Docs/Printer Part Codes.xlsx
+++ b/Docs/Printer Part Codes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jon\Documents\3D Print\Clockmaker\clock-3\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Repos\clock-3\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9205F57C-A4EA-4E11-8B09-E5B6EA4F2357}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAE8CF6E-4C33-4319-8F7C-72FAA28B8436}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23256" yWindow="0" windowWidth="22236" windowHeight="12960" xr2:uid="{7E6554FF-2F4B-4318-87E0-43D225F4F170}"/>
+    <workbookView xWindow="11424" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{7E6554FF-2F4B-4318-87E0-43D225F4F170}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="169">
   <si>
     <t>Component</t>
   </si>
@@ -514,6 +514,33 @@
   </si>
   <si>
     <t>85 - Electrical - Mount - 5A Buck Mount.stl</t>
+  </si>
+  <si>
+    <t>Exterior</t>
+  </si>
+  <si>
+    <t>100 - Exterior - Frame - Base Cap Type 1.stl</t>
+  </si>
+  <si>
+    <t>101 - Exterior - Frame - Base Cap Type 2.stl</t>
+  </si>
+  <si>
+    <t>Base Cap Type 2</t>
+  </si>
+  <si>
+    <t>Base Cap Type 1</t>
+  </si>
+  <si>
+    <t>Top Cap Type 1</t>
+  </si>
+  <si>
+    <t>102 - Exterior - Frame - Top Cap Type 1.stl</t>
+  </si>
+  <si>
+    <t>Top Cap Type 2</t>
+  </si>
+  <si>
+    <t>103 - Exterior - Frame - Top Cap Type 2.stl</t>
   </si>
 </sst>
 </file>
@@ -580,8 +607,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5F341AE2-224B-4051-B04D-BA10CC5651EC}" name="Table1" displayName="Table1" ref="A1:I70" totalsRowShown="0">
-  <autoFilter ref="A1:I70" xr:uid="{7A633D33-D295-46C3-AB03-03E2AB6E078E}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5F341AE2-224B-4051-B04D-BA10CC5651EC}" name="Table1" displayName="Table1" ref="A1:I74" totalsRowShown="0">
+  <autoFilter ref="A1:I74" xr:uid="{7A633D33-D295-46C3-AB03-03E2AB6E078E}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -907,26 +934,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CC8DB31-6D45-4FED-94B6-5390BD4B0F2C}">
-  <dimension ref="A1:I70"/>
+  <dimension ref="A1:I74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I61" sqref="I61"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I74" sqref="I74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" customWidth="1"/>
+    <col min="1" max="1" width="10.41796875" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1"/>
-    <col min="5" max="5" width="20.5703125" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" customWidth="1"/>
-    <col min="7" max="7" width="5.42578125" customWidth="1"/>
-    <col min="8" max="8" width="26.28515625" customWidth="1"/>
-    <col min="9" max="9" width="48.140625" customWidth="1"/>
+    <col min="3" max="3" width="16.15625" customWidth="1"/>
+    <col min="4" max="4" width="13.41796875" customWidth="1"/>
+    <col min="5" max="5" width="20.578125" customWidth="1"/>
+    <col min="6" max="6" width="11.26171875" customWidth="1"/>
+    <col min="7" max="7" width="5.41796875" customWidth="1"/>
+    <col min="8" max="8" width="26.26171875" customWidth="1"/>
+    <col min="9" max="9" width="48.15625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -955,7 +982,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -981,7 +1008,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1007,7 +1034,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1033,7 +1060,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1059,7 +1086,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1085,7 +1112,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1111,7 +1138,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1137,7 +1164,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1163,7 +1190,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1189,7 +1216,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1215,7 +1242,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1241,7 +1268,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1267,7 +1294,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1293,7 +1320,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1319,7 +1346,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1345,7 +1372,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1371,7 +1398,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1397,7 +1424,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1426,7 +1453,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1452,7 +1479,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1478,7 +1505,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1504,7 +1531,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1530,7 +1557,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1556,7 +1583,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1582,7 +1609,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1608,7 +1635,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1634,7 +1661,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1660,7 +1687,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1686,7 +1713,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1713,7 +1740,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1740,7 +1767,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1767,7 +1794,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1794,7 +1821,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1821,7 +1848,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1847,7 +1874,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1873,7 +1900,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A37">
         <v>41</v>
       </c>
@@ -1899,7 +1926,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A38">
         <v>42</v>
       </c>
@@ -1925,7 +1952,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A39">
         <v>43</v>
       </c>
@@ -1951,7 +1978,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A40">
         <v>44</v>
       </c>
@@ -1977,7 +2004,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A41">
         <v>45</v>
       </c>
@@ -2003,7 +2030,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A42">
         <v>51</v>
       </c>
@@ -2029,7 +2056,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A43">
         <v>60</v>
       </c>
@@ -2058,7 +2085,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A44">
         <v>61</v>
       </c>
@@ -2085,7 +2112,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A45">
         <v>62</v>
       </c>
@@ -2112,7 +2139,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A46">
         <v>70</v>
       </c>
@@ -2141,7 +2168,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A47">
         <v>71</v>
       </c>
@@ -2170,7 +2197,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A48">
         <v>72</v>
       </c>
@@ -2196,7 +2223,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A49">
         <v>73</v>
       </c>
@@ -2222,7 +2249,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A50">
         <v>74</v>
       </c>
@@ -2248,7 +2275,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A51">
         <v>75</v>
       </c>
@@ -2274,7 +2301,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A52">
         <v>76</v>
       </c>
@@ -2300,7 +2327,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A53">
         <v>77</v>
       </c>
@@ -2326,7 +2353,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A54">
         <v>78</v>
       </c>
@@ -2352,7 +2379,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A55">
         <v>79</v>
       </c>
@@ -2378,7 +2405,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A56">
         <v>80</v>
       </c>
@@ -2404,7 +2431,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A57">
         <v>81</v>
       </c>
@@ -2430,7 +2457,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A58">
         <v>82</v>
       </c>
@@ -2459,7 +2486,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A59">
         <v>83</v>
       </c>
@@ -2485,7 +2512,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A60">
         <v>84</v>
       </c>
@@ -2511,7 +2538,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A61">
         <v>85</v>
       </c>
@@ -2537,7 +2564,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A62">
         <v>90</v>
       </c>
@@ -2563,7 +2590,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A63">
         <v>91</v>
       </c>
@@ -2589,7 +2616,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A64">
         <v>92</v>
       </c>
@@ -2615,7 +2642,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A65">
         <v>93</v>
       </c>
@@ -2641,7 +2668,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A66">
         <v>94</v>
       </c>
@@ -2670,7 +2697,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A67">
         <v>95</v>
       </c>
@@ -2699,7 +2726,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A68">
         <v>96</v>
       </c>
@@ -2725,7 +2752,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A69">
         <v>97</v>
       </c>
@@ -2751,7 +2778,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A70">
         <v>98</v>
       </c>
@@ -2775,6 +2802,110 @@
       </c>
       <c r="I70" t="s">
         <v>150</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A71">
+        <v>100</v>
+      </c>
+      <c r="B71" t="s">
+        <v>160</v>
+      </c>
+      <c r="C71" t="s">
+        <v>40</v>
+      </c>
+      <c r="D71" t="s">
+        <v>1</v>
+      </c>
+      <c r="E71" t="s">
+        <v>164</v>
+      </c>
+      <c r="F71" t="s">
+        <v>56</v>
+      </c>
+      <c r="G71">
+        <v>2</v>
+      </c>
+      <c r="I71" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A72">
+        <v>101</v>
+      </c>
+      <c r="B72" t="s">
+        <v>160</v>
+      </c>
+      <c r="C72" t="s">
+        <v>40</v>
+      </c>
+      <c r="D72" t="s">
+        <v>1</v>
+      </c>
+      <c r="E72" t="s">
+        <v>163</v>
+      </c>
+      <c r="F72" t="s">
+        <v>56</v>
+      </c>
+      <c r="G72">
+        <v>2</v>
+      </c>
+      <c r="I72" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A73">
+        <v>102</v>
+      </c>
+      <c r="B73" t="s">
+        <v>160</v>
+      </c>
+      <c r="C73" t="s">
+        <v>40</v>
+      </c>
+      <c r="D73" t="s">
+        <v>1</v>
+      </c>
+      <c r="E73" t="s">
+        <v>165</v>
+      </c>
+      <c r="F73" t="s">
+        <v>56</v>
+      </c>
+      <c r="G73">
+        <v>2</v>
+      </c>
+      <c r="I73" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A74">
+        <v>103</v>
+      </c>
+      <c r="B74" t="s">
+        <v>160</v>
+      </c>
+      <c r="C74" t="s">
+        <v>40</v>
+      </c>
+      <c r="D74" t="s">
+        <v>1</v>
+      </c>
+      <c r="E74" t="s">
+        <v>167</v>
+      </c>
+      <c r="F74" t="s">
+        <v>56</v>
+      </c>
+      <c r="G74">
+        <v>2</v>
+      </c>
+      <c r="I74" t="s">
+        <v>168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
12/27 - Undercarriage and skirts work
- Finished rear exhaust and tagging pieces with IDs for the skirt.
- Publishing 104-111 and reserving 112 and 113 for the display (to be done when back in office).
- Fixed up the electronics undercarriage file with parts already designed.
- Added PSU to the model and desgined a power supply mount, as well.
</commit_message>
<xml_diff>
--- a/Docs/Printer Part Codes.xlsx
+++ b/Docs/Printer Part Codes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Repos\clock-3\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAE8CF6E-4C33-4319-8F7C-72FAA28B8436}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE266625-2761-480A-A025-5DAF43574436}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11424" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{7E6554FF-2F4B-4318-87E0-43D225F4F170}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="195">
   <si>
     <t>Component</t>
   </si>
@@ -541,6 +541,84 @@
   </si>
   <si>
     <t>103 - Exterior - Frame - Top Cap Type 2.stl</t>
+  </si>
+  <si>
+    <t>Skirt</t>
+  </si>
+  <si>
+    <t>L Front End</t>
+  </si>
+  <si>
+    <t>104 - Exterior - Skirt - L Front End.stl</t>
+  </si>
+  <si>
+    <t>R Front End</t>
+  </si>
+  <si>
+    <t>105 - Exterior - Skirt - R Front End.stl</t>
+  </si>
+  <si>
+    <t>L Rear End</t>
+  </si>
+  <si>
+    <t>106 - Exterior - Skirt - L Rear End.stl</t>
+  </si>
+  <si>
+    <t>R Rear End</t>
+  </si>
+  <si>
+    <t>107 - Exterior - Skirt - R Rear End.stl</t>
+  </si>
+  <si>
+    <t>108 - Exterior - Skirt - Grille.stl</t>
+  </si>
+  <si>
+    <t>Grille</t>
+  </si>
+  <si>
+    <t>110 - Exterior - Skirt - Fan Intake.stl</t>
+  </si>
+  <si>
+    <t>Fan Exhuast</t>
+  </si>
+  <si>
+    <t>Interchangeable with 110</t>
+  </si>
+  <si>
+    <t>Interchangeable with 111</t>
+  </si>
+  <si>
+    <t>Screen Mount</t>
+  </si>
+  <si>
+    <t>111 - Exterior - Skirt - Fan Exhaust.stl</t>
+  </si>
+  <si>
+    <t>92mm Fan Mount</t>
+  </si>
+  <si>
+    <t>109 - Exterior - Skirt - 92mm Fan Mount.stl</t>
+  </si>
+  <si>
+    <t>IEC (power) plug</t>
+  </si>
+  <si>
+    <t>Power switch</t>
+  </si>
+  <si>
+    <t>Screen Adapter</t>
+  </si>
+  <si>
+    <t>113 - Exterior - Skirt - Screen Adapter.stl</t>
+  </si>
+  <si>
+    <t>112 - Exterior - Skirt - Screen Mount.stl</t>
+  </si>
+  <si>
+    <t>PSU Mount</t>
+  </si>
+  <si>
+    <t>86 - Electrical - Mount - PSU Mount.stl</t>
   </si>
 </sst>
 </file>
@@ -607,8 +685,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5F341AE2-224B-4051-B04D-BA10CC5651EC}" name="Table1" displayName="Table1" ref="A1:I74" totalsRowShown="0">
-  <autoFilter ref="A1:I74" xr:uid="{7A633D33-D295-46C3-AB03-03E2AB6E078E}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5F341AE2-224B-4051-B04D-BA10CC5651EC}" name="Table1" displayName="Table1" ref="A1:I85" totalsRowShown="0">
+  <autoFilter ref="A1:I85" xr:uid="{7A633D33-D295-46C3-AB03-03E2AB6E078E}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -619,8 +697,8 @@
     <filterColumn colId="7" hiddenButton="1"/>
     <filterColumn colId="8" hiddenButton="1"/>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I68">
-    <sortCondition ref="A1:A68"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I69">
+    <sortCondition ref="A1:A69"/>
   </sortState>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{A8EA61BD-839A-4759-B873-CEDA7BEA684B}" name="Number"/>
@@ -934,10 +1012,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CC8DB31-6D45-4FED-94B6-5390BD4B0F2C}">
-  <dimension ref="A1:I74"/>
+  <dimension ref="A1:I85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I74" sqref="I74"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F77" sqref="F77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2566,169 +2644,166 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A62">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B62" t="s">
-        <v>37</v>
+        <v>119</v>
       </c>
       <c r="C62" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="D62" t="s">
         <v>1</v>
       </c>
       <c r="E62" t="s">
-        <v>38</v>
+        <v>193</v>
       </c>
       <c r="F62" t="s">
         <v>56</v>
       </c>
-      <c r="G62" t="s">
-        <v>61</v>
+      <c r="G62">
+        <v>2</v>
       </c>
       <c r="I62" t="s">
-        <v>114</v>
+        <v>194</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A63">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B63" t="s">
         <v>37</v>
       </c>
       <c r="C63" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="D63" t="s">
         <v>1</v>
       </c>
       <c r="E63" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F63" t="s">
         <v>56</v>
       </c>
-      <c r="G63">
-        <v>5</v>
+      <c r="G63" t="s">
+        <v>61</v>
       </c>
       <c r="I63" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A64">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B64" t="s">
         <v>37</v>
       </c>
       <c r="C64" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="D64" t="s">
         <v>1</v>
       </c>
       <c r="E64" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F64" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="G64">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I64" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A65">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B65" t="s">
+        <v>37</v>
+      </c>
+      <c r="C65" t="s">
+        <v>40</v>
+      </c>
+      <c r="D65" t="s">
+        <v>1</v>
+      </c>
+      <c r="E65" t="s">
+        <v>41</v>
+      </c>
+      <c r="F65" t="s">
+        <v>36</v>
+      </c>
+      <c r="G65">
         <v>4</v>
       </c>
-      <c r="C65" t="s">
-        <v>25</v>
-      </c>
-      <c r="D65" t="s">
-        <v>9</v>
-      </c>
-      <c r="E65" t="s">
-        <v>59</v>
-      </c>
-      <c r="F65" t="s">
-        <v>56</v>
-      </c>
-      <c r="G65">
-        <v>1</v>
-      </c>
       <c r="I65" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A66">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B66" t="s">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="C66" t="s">
-        <v>68</v>
+        <v>25</v>
       </c>
       <c r="D66" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E66" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="F66" t="s">
         <v>56</v>
       </c>
       <c r="G66">
-        <v>2</v>
-      </c>
-      <c r="H66" t="s">
-        <v>133</v>
+        <v>1</v>
       </c>
       <c r="I66" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A67">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B67" t="s">
         <v>37</v>
       </c>
       <c r="C67" t="s">
-        <v>120</v>
+        <v>68</v>
       </c>
       <c r="D67" t="s">
         <v>1</v>
       </c>
       <c r="E67" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="F67" t="s">
-        <v>36</v>
-      </c>
-      <c r="G67" t="s">
-        <v>61</v>
+        <v>56</v>
+      </c>
+      <c r="G67">
+        <v>2</v>
       </c>
       <c r="H67" t="s">
         <v>133</v>
       </c>
       <c r="I67" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A68">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B68" t="s">
         <v>37</v>
@@ -2740,21 +2815,24 @@
         <v>1</v>
       </c>
       <c r="E68" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="F68" t="s">
-        <v>56</v>
-      </c>
-      <c r="G68">
-        <v>10</v>
+        <v>36</v>
+      </c>
+      <c r="G68" t="s">
+        <v>61</v>
+      </c>
+      <c r="H68" t="s">
+        <v>133</v>
       </c>
       <c r="I68" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A69">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B69" t="s">
         <v>37</v>
@@ -2763,24 +2841,24 @@
         <v>120</v>
       </c>
       <c r="D69" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E69" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F69" t="s">
         <v>56</v>
       </c>
       <c r="G69">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="I69" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A70">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B70" t="s">
         <v>37</v>
@@ -2789,10 +2867,10 @@
         <v>120</v>
       </c>
       <c r="D70" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E70" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="F70" t="s">
         <v>56</v>
@@ -2801,38 +2879,38 @@
         <v>1</v>
       </c>
       <c r="I70" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A71">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B71" t="s">
-        <v>160</v>
+        <v>37</v>
       </c>
       <c r="C71" t="s">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="D71" t="s">
         <v>1</v>
       </c>
       <c r="E71" t="s">
-        <v>164</v>
+        <v>149</v>
       </c>
       <c r="F71" t="s">
         <v>56</v>
       </c>
       <c r="G71">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I71" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A72">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B72" t="s">
         <v>160</v>
@@ -2844,7 +2922,7 @@
         <v>1</v>
       </c>
       <c r="E72" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="F72" t="s">
         <v>56</v>
@@ -2853,12 +2931,12 @@
         <v>2</v>
       </c>
       <c r="I72" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A73">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B73" t="s">
         <v>160</v>
@@ -2870,7 +2948,7 @@
         <v>1</v>
       </c>
       <c r="E73" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F73" t="s">
         <v>56</v>
@@ -2879,12 +2957,12 @@
         <v>2</v>
       </c>
       <c r="I73" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A74">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B74" t="s">
         <v>160</v>
@@ -2896,7 +2974,7 @@
         <v>1</v>
       </c>
       <c r="E74" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F74" t="s">
         <v>56</v>
@@ -2905,7 +2983,305 @@
         <v>2</v>
       </c>
       <c r="I74" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A75">
+        <v>103</v>
+      </c>
+      <c r="B75" t="s">
+        <v>160</v>
+      </c>
+      <c r="C75" t="s">
+        <v>40</v>
+      </c>
+      <c r="D75" t="s">
+        <v>1</v>
+      </c>
+      <c r="E75" t="s">
+        <v>167</v>
+      </c>
+      <c r="F75" t="s">
+        <v>56</v>
+      </c>
+      <c r="G75">
+        <v>2</v>
+      </c>
+      <c r="I75" t="s">
         <v>168</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A76">
+        <v>104</v>
+      </c>
+      <c r="B76" t="s">
+        <v>160</v>
+      </c>
+      <c r="C76" t="s">
+        <v>169</v>
+      </c>
+      <c r="D76" t="s">
+        <v>5</v>
+      </c>
+      <c r="E76" t="s">
+        <v>170</v>
+      </c>
+      <c r="F76" t="s">
+        <v>56</v>
+      </c>
+      <c r="G76">
+        <v>1</v>
+      </c>
+      <c r="I76" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A77">
+        <v>105</v>
+      </c>
+      <c r="B77" t="s">
+        <v>160</v>
+      </c>
+      <c r="C77" t="s">
+        <v>169</v>
+      </c>
+      <c r="D77" t="s">
+        <v>9</v>
+      </c>
+      <c r="E77" t="s">
+        <v>172</v>
+      </c>
+      <c r="F77" t="s">
+        <v>56</v>
+      </c>
+      <c r="G77">
+        <v>1</v>
+      </c>
+      <c r="H77" t="s">
+        <v>189</v>
+      </c>
+      <c r="I77" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A78">
+        <v>106</v>
+      </c>
+      <c r="B78" t="s">
+        <v>160</v>
+      </c>
+      <c r="C78" t="s">
+        <v>169</v>
+      </c>
+      <c r="D78" t="s">
+        <v>5</v>
+      </c>
+      <c r="E78" t="s">
+        <v>174</v>
+      </c>
+      <c r="F78" t="s">
+        <v>56</v>
+      </c>
+      <c r="G78">
+        <v>1</v>
+      </c>
+      <c r="I78" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A79">
+        <v>107</v>
+      </c>
+      <c r="B79" t="s">
+        <v>160</v>
+      </c>
+      <c r="C79" t="s">
+        <v>169</v>
+      </c>
+      <c r="D79" t="s">
+        <v>9</v>
+      </c>
+      <c r="E79" t="s">
+        <v>176</v>
+      </c>
+      <c r="F79" t="s">
+        <v>56</v>
+      </c>
+      <c r="G79">
+        <v>1</v>
+      </c>
+      <c r="H79" t="s">
+        <v>188</v>
+      </c>
+      <c r="I79" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A80">
+        <v>108</v>
+      </c>
+      <c r="B80" t="s">
+        <v>160</v>
+      </c>
+      <c r="C80" t="s">
+        <v>169</v>
+      </c>
+      <c r="D80" t="s">
+        <v>1</v>
+      </c>
+      <c r="E80" t="s">
+        <v>179</v>
+      </c>
+      <c r="F80" t="s">
+        <v>56</v>
+      </c>
+      <c r="G80">
+        <v>4</v>
+      </c>
+      <c r="I80" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A81">
+        <v>109</v>
+      </c>
+      <c r="B81" t="s">
+        <v>160</v>
+      </c>
+      <c r="C81" t="s">
+        <v>169</v>
+      </c>
+      <c r="D81" t="s">
+        <v>1</v>
+      </c>
+      <c r="E81" t="s">
+        <v>186</v>
+      </c>
+      <c r="F81" t="s">
+        <v>56</v>
+      </c>
+      <c r="G81">
+        <v>3</v>
+      </c>
+      <c r="I81" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A82">
+        <v>110</v>
+      </c>
+      <c r="B82" t="s">
+        <v>160</v>
+      </c>
+      <c r="C82" t="s">
+        <v>169</v>
+      </c>
+      <c r="D82" t="s">
+        <v>1</v>
+      </c>
+      <c r="E82" t="s">
+        <v>34</v>
+      </c>
+      <c r="F82" t="s">
+        <v>56</v>
+      </c>
+      <c r="G82">
+        <v>1</v>
+      </c>
+      <c r="H82" t="s">
+        <v>183</v>
+      </c>
+      <c r="I82" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A83">
+        <v>111</v>
+      </c>
+      <c r="B83" t="s">
+        <v>160</v>
+      </c>
+      <c r="C83" t="s">
+        <v>169</v>
+      </c>
+      <c r="D83" t="s">
+        <v>1</v>
+      </c>
+      <c r="E83" t="s">
+        <v>181</v>
+      </c>
+      <c r="F83" t="s">
+        <v>56</v>
+      </c>
+      <c r="G83">
+        <v>2</v>
+      </c>
+      <c r="H83" t="s">
+        <v>182</v>
+      </c>
+      <c r="I83" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A84">
+        <v>112</v>
+      </c>
+      <c r="B84" t="s">
+        <v>160</v>
+      </c>
+      <c r="C84" t="s">
+        <v>169</v>
+      </c>
+      <c r="D84" t="s">
+        <v>1</v>
+      </c>
+      <c r="E84" t="s">
+        <v>184</v>
+      </c>
+      <c r="F84" t="s">
+        <v>56</v>
+      </c>
+      <c r="G84">
+        <v>1</v>
+      </c>
+      <c r="I84" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A85">
+        <v>113</v>
+      </c>
+      <c r="B85" t="s">
+        <v>160</v>
+      </c>
+      <c r="C85" t="s">
+        <v>169</v>
+      </c>
+      <c r="D85" t="s">
+        <v>1</v>
+      </c>
+      <c r="E85" t="s">
+        <v>190</v>
+      </c>
+      <c r="F85" t="s">
+        <v>56</v>
+      </c>
+      <c r="G85">
+        <v>1</v>
+      </c>
+      <c r="I85" t="s">
+        <v>191</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
12/29 & 12/30 - Many fixes; see changelog
## 2021-12-30

- Added some bracing to the electrical panel mounts to reduce flex and moved them further back.
- Introduced the wiring panels to the master model.
- Added lighting into the model for 3 x 12 pixel strips at 60px/m (16.6mm spacing).
- Made a few fixes to the lighting strip so the zip tie does not cross over an LED.
- Plenty of new renders.

## 2021-12-29

- Fixed ABL mount issues with belt attachment screws.
- Also simplified mounting the hotend fan. Two screws mount into the fan shroud and two pass through to mount both. The fan shroud and fan then can come off with two screws instead of four.
- Added motion joints.
- Reviewed assemblies and added any missing fasteners.
- Updated wiring anchors on the x gantry. BMG mount now has a groove and zip tie channels for wiring on the right side.
- `Electrical T Slot Extension` now has a slot for inserting new roll-in tee nuts (or taking them out) without having to dismount the extrusion.
</commit_message>
<xml_diff>
--- a/Docs/Printer Part Codes.xlsx
+++ b/Docs/Printer Part Codes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Repos\clock-3\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A834F0E-032E-4227-9184-96857B9280B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49784819-83AB-46DA-888C-8271600ABB41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11424" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{7E6554FF-2F4B-4318-87E0-43D225F4F170}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="194">
   <si>
     <t>Component</t>
   </si>
@@ -385,12 +385,6 @@
   </si>
   <si>
     <t>75 - Electrical - Wiring - L Panel Faceplate.stl</t>
-  </si>
-  <si>
-    <t>Wire Guide</t>
-  </si>
-  <si>
-    <t>95 - Misc - Wiring - Wire Guide.stl</t>
   </si>
   <si>
     <t>Still Testing</t>
@@ -688,10 +682,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5F341AE2-224B-4051-B04D-BA10CC5651EC}" name="Table1" displayName="Table1" ref="A1:I85" totalsRowShown="0">
-  <autoFilter ref="A1:I85" xr:uid="{7A633D33-D295-46C3-AB03-03E2AB6E078E}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I85">
-    <sortCondition ref="A1:A85"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5F341AE2-224B-4051-B04D-BA10CC5651EC}" name="Table1" displayName="Table1" ref="A1:I84" totalsRowShown="0">
+  <autoFilter ref="A1:I84" xr:uid="{7A633D33-D295-46C3-AB03-03E2AB6E078E}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I84">
+    <sortCondition ref="A1:A84"/>
   </sortState>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{A8EA61BD-839A-4759-B873-CEDA7BEA684B}" name="Number"/>
@@ -1005,10 +999,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CC8DB31-6D45-4FED-94B6-5390BD4B0F2C}">
-  <dimension ref="A1:I85"/>
+  <dimension ref="A1:I84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F75" sqref="F75"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H60" sqref="H60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1431,7 +1425,7 @@
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="F16" t="s">
         <v>35</v>
@@ -1440,10 +1434,10 @@
         <v>2</v>
       </c>
       <c r="H16" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="I16" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -1838,7 +1832,7 @@
       </c>
       <c r="H31" s="1"/>
       <c r="I31" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -1865,7 +1859,7 @@
       </c>
       <c r="H32" s="1"/>
       <c r="I32" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -1892,7 +1886,7 @@
       </c>
       <c r="H33" s="1"/>
       <c r="I33" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -1919,7 +1913,7 @@
       </c>
       <c r="H34" s="1"/>
       <c r="I34" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -1988,7 +1982,7 @@
         <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F37" t="s">
         <v>55</v>
@@ -1997,7 +1991,7 @@
         <v>1</v>
       </c>
       <c r="I37" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -2023,7 +2017,7 @@
         <v>1</v>
       </c>
       <c r="I38" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -2049,7 +2043,7 @@
         <v>1</v>
       </c>
       <c r="I39" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -2075,7 +2069,7 @@
         <v>1</v>
       </c>
       <c r="I40" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -2164,7 +2158,7 @@
         <v>46</v>
       </c>
       <c r="C44" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D44" t="s">
         <v>1</v>
@@ -2182,7 +2176,7 @@
         <v>63</v>
       </c>
       <c r="I44" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -2193,7 +2187,7 @@
         <v>46</v>
       </c>
       <c r="C45" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D45" t="s">
         <v>1</v>
@@ -2209,7 +2203,7 @@
       </c>
       <c r="H45" s="1"/>
       <c r="I45" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
@@ -2220,7 +2214,7 @@
         <v>46</v>
       </c>
       <c r="C46" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D46" t="s">
         <v>1</v>
@@ -2236,7 +2230,7 @@
       </c>
       <c r="H46" s="1"/>
       <c r="I46" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
@@ -2415,16 +2409,16 @@
         <v>5</v>
       </c>
       <c r="E53" t="s">
+        <v>121</v>
+      </c>
+      <c r="F53" t="s">
+        <v>55</v>
+      </c>
+      <c r="G53">
+        <v>1</v>
+      </c>
+      <c r="I53" t="s">
         <v>123</v>
-      </c>
-      <c r="F53" t="s">
-        <v>55</v>
-      </c>
-      <c r="G53">
-        <v>1</v>
-      </c>
-      <c r="I53" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
@@ -2441,7 +2435,7 @@
         <v>9</v>
       </c>
       <c r="E54" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F54" t="s">
         <v>55</v>
@@ -2450,7 +2444,7 @@
         <v>1</v>
       </c>
       <c r="I54" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
@@ -2467,7 +2461,7 @@
         <v>5</v>
       </c>
       <c r="E55" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F55" t="s">
         <v>55</v>
@@ -2476,7 +2470,7 @@
         <v>1</v>
       </c>
       <c r="I55" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
@@ -2493,7 +2487,7 @@
         <v>9</v>
       </c>
       <c r="E56" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F56" t="s">
         <v>55</v>
@@ -2502,7 +2496,7 @@
         <v>1</v>
       </c>
       <c r="I56" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
@@ -2519,7 +2513,7 @@
         <v>1</v>
       </c>
       <c r="E57" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F57" t="s">
         <v>55</v>
@@ -2528,7 +2522,7 @@
         <v>1</v>
       </c>
       <c r="I57" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
@@ -2539,22 +2533,22 @@
         <v>105</v>
       </c>
       <c r="C58" t="s">
+        <v>127</v>
+      </c>
+      <c r="D58" t="s">
+        <v>1</v>
+      </c>
+      <c r="E58" t="s">
+        <v>128</v>
+      </c>
+      <c r="F58" t="s">
+        <v>55</v>
+      </c>
+      <c r="G58">
+        <v>1</v>
+      </c>
+      <c r="I58" t="s">
         <v>129</v>
-      </c>
-      <c r="D58" t="s">
-        <v>1</v>
-      </c>
-      <c r="E58" t="s">
-        <v>130</v>
-      </c>
-      <c r="F58" t="s">
-        <v>55</v>
-      </c>
-      <c r="G58">
-        <v>1</v>
-      </c>
-      <c r="I58" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
@@ -2565,25 +2559,25 @@
         <v>105</v>
       </c>
       <c r="C59" t="s">
+        <v>133</v>
+      </c>
+      <c r="D59" t="s">
+        <v>1</v>
+      </c>
+      <c r="E59" t="s">
+        <v>136</v>
+      </c>
+      <c r="F59" t="s">
+        <v>55</v>
+      </c>
+      <c r="G59">
+        <v>1</v>
+      </c>
+      <c r="H59" t="s">
+        <v>134</v>
+      </c>
+      <c r="I59" t="s">
         <v>135</v>
-      </c>
-      <c r="D59" t="s">
-        <v>1</v>
-      </c>
-      <c r="E59" t="s">
-        <v>138</v>
-      </c>
-      <c r="F59" t="s">
-        <v>55</v>
-      </c>
-      <c r="G59">
-        <v>1</v>
-      </c>
-      <c r="H59" t="s">
-        <v>136</v>
-      </c>
-      <c r="I59" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
@@ -2600,7 +2594,7 @@
         <v>5</v>
       </c>
       <c r="E60" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F60" t="s">
         <v>55</v>
@@ -2609,7 +2603,7 @@
         <v>1</v>
       </c>
       <c r="I60" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
@@ -2626,16 +2620,16 @@
         <v>9</v>
       </c>
       <c r="E61" t="s">
+        <v>137</v>
+      </c>
+      <c r="F61" t="s">
+        <v>55</v>
+      </c>
+      <c r="G61">
+        <v>1</v>
+      </c>
+      <c r="I61" t="s">
         <v>139</v>
-      </c>
-      <c r="F61" t="s">
-        <v>55</v>
-      </c>
-      <c r="G61">
-        <v>1</v>
-      </c>
-      <c r="I61" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
@@ -2652,7 +2646,7 @@
         <v>1</v>
       </c>
       <c r="E62" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F62" t="s">
         <v>55</v>
@@ -2661,7 +2655,7 @@
         <v>1</v>
       </c>
       <c r="I62" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
@@ -2678,7 +2672,7 @@
         <v>1</v>
       </c>
       <c r="E63" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F63" t="s">
         <v>55</v>
@@ -2687,7 +2681,7 @@
         <v>2</v>
       </c>
       <c r="I63" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
@@ -2817,7 +2811,7 @@
         <v>2</v>
       </c>
       <c r="H68" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="I68" t="s">
         <v>104</v>
@@ -2825,7 +2819,7 @@
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B69" t="s">
         <v>36</v>
@@ -2837,24 +2831,21 @@
         <v>1</v>
       </c>
       <c r="E69" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="F69" t="s">
-        <v>35</v>
-      </c>
-      <c r="G69" t="s">
-        <v>60</v>
-      </c>
-      <c r="H69" t="s">
+        <v>55</v>
+      </c>
+      <c r="G69">
+        <v>10</v>
+      </c>
+      <c r="I69" t="s">
         <v>119</v>
-      </c>
-      <c r="I69" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B70" t="s">
         <v>36</v>
@@ -2866,50 +2857,50 @@
         <v>1</v>
       </c>
       <c r="E70" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="F70" t="s">
         <v>55</v>
       </c>
       <c r="G70">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="I70" t="s">
-        <v>121</v>
+        <v>132</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B71" t="s">
-        <v>36</v>
+        <v>142</v>
       </c>
       <c r="C71" t="s">
-        <v>106</v>
+        <v>39</v>
       </c>
       <c r="D71" t="s">
         <v>1</v>
       </c>
       <c r="E71" t="s">
-        <v>133</v>
+        <v>146</v>
       </c>
       <c r="F71" t="s">
         <v>55</v>
       </c>
       <c r="G71">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I71" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B72" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C72" t="s">
         <v>39</v>
@@ -2918,7 +2909,7 @@
         <v>1</v>
       </c>
       <c r="E72" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="F72" t="s">
         <v>55</v>
@@ -2927,15 +2918,15 @@
         <v>2</v>
       </c>
       <c r="I72" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B73" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C73" t="s">
         <v>39</v>
@@ -2953,15 +2944,15 @@
         <v>2</v>
       </c>
       <c r="I73" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B74" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C74" t="s">
         <v>39</v>
@@ -2984,42 +2975,42 @@
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B75" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C75" t="s">
-        <v>39</v>
+        <v>151</v>
       </c>
       <c r="D75" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E75" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F75" t="s">
         <v>55</v>
       </c>
       <c r="G75">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I75" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B76" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C76" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D76" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E76" t="s">
         <v>154</v>
@@ -3030,22 +3021,25 @@
       <c r="G76">
         <v>1</v>
       </c>
+      <c r="H76" t="s">
+        <v>171</v>
+      </c>
       <c r="I76" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B77" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C77" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D77" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E77" t="s">
         <v>156</v>
@@ -3056,25 +3050,22 @@
       <c r="G77">
         <v>1</v>
       </c>
-      <c r="H77" t="s">
-        <v>173</v>
-      </c>
       <c r="I77" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B78" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C78" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D78" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E78" t="s">
         <v>158</v>
@@ -3085,164 +3076,164 @@
       <c r="G78">
         <v>1</v>
       </c>
+      <c r="H78" t="s">
+        <v>170</v>
+      </c>
       <c r="I78" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B79" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C79" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D79" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E79" t="s">
+        <v>161</v>
+      </c>
+      <c r="F79" t="s">
+        <v>55</v>
+      </c>
+      <c r="G79">
+        <v>4</v>
+      </c>
+      <c r="I79" t="s">
         <v>160</v>
-      </c>
-      <c r="F79" t="s">
-        <v>55</v>
-      </c>
-      <c r="G79">
-        <v>1</v>
-      </c>
-      <c r="H79" t="s">
-        <v>172</v>
-      </c>
-      <c r="I79" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B80" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C80" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D80" t="s">
         <v>1</v>
       </c>
       <c r="E80" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="F80" t="s">
         <v>55</v>
       </c>
       <c r="G80">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I80" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B81" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C81" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D81" t="s">
         <v>1</v>
       </c>
       <c r="E81" t="s">
-        <v>170</v>
+        <v>33</v>
       </c>
       <c r="F81" t="s">
         <v>55</v>
       </c>
       <c r="G81">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="H81" t="s">
+        <v>165</v>
       </c>
       <c r="I81" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B82" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C82" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D82" t="s">
         <v>1</v>
       </c>
       <c r="E82" t="s">
-        <v>33</v>
+        <v>163</v>
       </c>
       <c r="F82" t="s">
         <v>55</v>
       </c>
       <c r="G82">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H82" t="s">
+        <v>164</v>
+      </c>
+      <c r="I82" t="s">
         <v>167</v>
-      </c>
-      <c r="I82" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B83" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C83" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D83" t="s">
         <v>1</v>
       </c>
       <c r="E83" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F83" t="s">
         <v>55</v>
       </c>
       <c r="G83">
-        <v>2</v>
-      </c>
-      <c r="H83" t="s">
-        <v>166</v>
+        <v>1</v>
       </c>
       <c r="I83" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B84" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C84" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D84" t="s">
         <v>1</v>
       </c>
       <c r="E84" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="F84" t="s">
         <v>55</v>
@@ -3251,33 +3242,7 @@
         <v>1</v>
       </c>
       <c r="I84" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A85">
-        <v>113</v>
-      </c>
-      <c r="B85" t="s">
-        <v>144</v>
-      </c>
-      <c r="C85" t="s">
-        <v>153</v>
-      </c>
-      <c r="D85" t="s">
-        <v>1</v>
-      </c>
-      <c r="E85" t="s">
-        <v>174</v>
-      </c>
-      <c r="F85" t="s">
-        <v>55</v>
-      </c>
-      <c r="G85">
-        <v>1</v>
-      </c>
-      <c r="I85" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pushing current filtration work
- Made shims/TPU gaskets for both 75mm and 50mm fans. They push the fans out 1.6mm to make room for a hose adapter (and dampen noise).
- Both the 50mm and 75mm fan intakes work, though the right 50mm profile is incorrect.
- Working on 75mm fan exhaust to tighten fit. Modeling is difficult as there is some variation between brands in wall thicknesses, etc.
- Ordered 1" ID hose instead of 1/4". The 75mm fan is having difficulty providing pressure, so I'm going to try avoiding necking down. The 1/4" hosing may still be useful for 50mm fans.
- 1/4" hose is ideal for 50mm fan.
- 50mm fan intake is now front heavy with hose on, added hole for an insert and foot.
- Started work on a fully vertical filter tower.
</commit_message>
<xml_diff>
--- a/Docs/Printer Part Codes.xlsx
+++ b/Docs/Printer Part Codes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jon\Documents\3D Print\Clockmaker\clock-3\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3C92C89F-7627-4C27-9C45-2C31CA16F9C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C1892D0-F183-490F-AAAC-236D72221DAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{7E6554FF-2F4B-4318-87E0-43D225F4F170}"/>
   </bookViews>
@@ -1009,7 +1009,7 @@
   <dimension ref="A1:I85"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I65" sqref="I65"/>
+      <selection activeCell="H59" sqref="H59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>